<commit_message>
Fun Formula to Unstack Columns
I really enjoyed this one. I hate unstacking arrays. This creates a function to do that.
</commit_message>
<xml_diff>
--- a/UnwrapAnArray.xlsx
+++ b/UnwrapAnArray.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{08AD3DBE-035A-406A-9BB9-F1005714D6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFC58DF3-05B8-4A29-880B-2D421FE8E49F}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{08AD3DBE-035A-406A-9BB9-F1005714D6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19BB00B7-B074-4470-BFA3-02D011E1E454}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="2" r:id="rId1"/>
     <sheet name="InterestingFormula" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Table1!$A$1:$F$6</definedName>
+    <definedName name="SplitCols">_xlfn.LAMBDA(_xlpm.array,_xlpm.start,_xlpm.end,_xlfn.TAKE(_xlfn.DROP(_xlpm.array,,_xlpm.start-1),,_xlpm.end-_xlpm.start+1))</definedName>
+    <definedName name="Stacker">_xlfn.LAMBDA(_xlpm.array,_xlfn.DROP(_xlfn.REDUCE({0,0},_xlfn.SEQUENCE(,COLUMNS(_xlpm.array)/2,1,2),_xlfn.LAMBDA(_xlpm.x,_xlpm.y, _xlfn.VSTACK(_xlpm.x,SplitCols(_xlpm.array,_xlpm.y,_xlpm.y+1)))),1))</definedName>
+    <definedName name="Stacker2">_xlfn.LAMBDA(_xlpm.array,_xlpm.cols,    _xlfn.DROP(      _xlfn.REDUCE(        _xlfn.SEQUENCE(,_xlpm.cols,0,0),        _xlfn.SEQUENCE(          ,          COLUMNS(            _xlpm.array)/_xlpm.cols,1,_xlpm.cols),        _xlfn.LAMBDA(_xlpm.x,_xlpm.y,          _xlfn.VSTACK(            _xlpm.x,            SplitCols(              _xlpm.array,_xlpm.y,_xlpm.y+_xlpm.cols-1)))),1))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,8 +53,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -59,16 +66,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>FROM:</t>
   </si>
@@ -179,6 +200,72 @@
   </si>
   <si>
     <t>This is an amazing formula</t>
+  </si>
+  <si>
+    <t>Another Approach</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
+  </si>
+  <si>
+    <t>Col5</t>
+  </si>
+  <si>
+    <t>Col6</t>
+  </si>
+  <si>
+    <t>Col7</t>
+  </si>
+  <si>
+    <t>Col8</t>
+  </si>
+  <si>
+    <t>zz</t>
+  </si>
+  <si>
+    <t>Col9</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>Col10</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>Col11</t>
+  </si>
+  <si>
+    <t>yy</t>
+  </si>
+  <si>
+    <t>Col12</t>
+  </si>
+  <si>
+    <t>Arbitrary Length Column Stacker</t>
   </si>
 </sst>
 </file>
@@ -354,12 +441,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -492,6 +580,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>478478</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>135634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60468252-6813-B7C7-FBB9-F28479B51DCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="1552575"/>
+          <a:ext cx="2314898" cy="2715004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{ACF7C038-5484-4869-AB91-353963F8D109}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
@@ -505,6 +642,68 @@
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>1</v>
+    <v>8</v>
+    <v>17</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -532,6 +731,27 @@
     <tableColumn id="4" xr3:uid="{E5CFCDA3-092B-4946-A613-936AF4E7BCF8}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{8CD3CD0B-AF73-496A-A2E6-5BBDD58CA3A2}" name="Column5"/>
     <tableColumn id="6" xr3:uid="{5B5563BB-6EC5-44F4-9F8D-552B0587F99B}" name="Column6"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD08A751-79EA-4BFB-9F9B-07C13AEF146D}" name="_tTest" displayName="_tTest" ref="C9:N12" totalsRowShown="0">
+  <autoFilter ref="C9:N12" xr:uid="{FD08A751-79EA-4BFB-9F9B-07C13AEF146D}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{6A3ECD6A-6153-4707-BAA3-D899FDC4675C}" name="Col1"/>
+    <tableColumn id="2" xr3:uid="{09710337-57C1-4968-8FAE-DD7999C32D0F}" name="Col2"/>
+    <tableColumn id="3" xr3:uid="{DB033F19-D366-4FDC-8B25-B6D68DE08D10}" name="Col3"/>
+    <tableColumn id="4" xr3:uid="{7EA57B84-0BCB-4D15-A4FC-9A6E137C3626}" name="Col4"/>
+    <tableColumn id="5" xr3:uid="{4E9D5E1C-23A1-4086-8F0A-84FAAB04B877}" name="Col5"/>
+    <tableColumn id="6" xr3:uid="{CCB1E340-9993-421F-8C6E-A95C0362B5E4}" name="Col6"/>
+    <tableColumn id="7" xr3:uid="{73A05192-4A81-4BA6-ABEB-53F050AB6A7D}" name="Col7"/>
+    <tableColumn id="8" xr3:uid="{56C4ECA5-1431-49A1-AF19-90F772EAA41E}" name="Col8"/>
+    <tableColumn id="9" xr3:uid="{9F2A1237-BDFD-4729-A42B-FD08823948D5}" name="Col9"/>
+    <tableColumn id="10" xr3:uid="{A1B4D0C5-0C7B-4101-8A1A-5970BAE81642}" name="Col10"/>
+    <tableColumn id="11" xr3:uid="{B60DC55E-800B-49B9-9262-E42DB981178B}" name="Col11"/>
+    <tableColumn id="12" xr3:uid="{64AB61C1-44B6-4CF6-ADC8-3187DBE6D981}" name="Col12"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -870,8 +1090,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="AA48" sqref="AA48"/>
+    <sheetView topLeftCell="K16" workbookViewId="0">
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="V27">
-        <f>(S27-1)*4</f>
+        <f t="shared" ref="V27:V38" si="0">(S27-1)*4</f>
         <v>0</v>
       </c>
       <c r="W27">
@@ -1240,11 +1460,11 @@
         <v>2</v>
       </c>
       <c r="V28">
-        <f>(S28-1)*4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W28">
-        <f t="shared" ref="W28:W38" si="0">U28-V28</f>
+        <f t="shared" ref="W28:W38" si="1">U28-V28</f>
         <v>2</v>
       </c>
     </row>
@@ -1265,11 +1485,11 @@
         <v>3</v>
       </c>
       <c r="V29">
-        <f>(S29-1)*4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1297,11 +1517,11 @@
         <v>4</v>
       </c>
       <c r="V30">
-        <f>(S30-1)*4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1328,11 +1548,11 @@
         <v>5</v>
       </c>
       <c r="V31">
-        <f>(S31-1)*4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="W31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1359,11 +1579,11 @@
         <v>6</v>
       </c>
       <c r="V32">
-        <f>(S32-1)*4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="W32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1390,11 +1610,11 @@
         <v>7</v>
       </c>
       <c r="V33">
-        <f>(S33-1)*4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="W33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1421,11 +1641,11 @@
         <v>8</v>
       </c>
       <c r="V34">
-        <f>(S34-1)*4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="W34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1452,11 +1672,11 @@
         <v>9</v>
       </c>
       <c r="V35">
-        <f>(S35-1)*4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="W35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1483,11 +1703,11 @@
         <v>10</v>
       </c>
       <c r="V36">
-        <f>(S36-1)*4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="W36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1511,11 +1731,11 @@
         <v>11</v>
       </c>
       <c r="V37">
-        <f>(S37-1)*4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="W37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1533,11 +1753,11 @@
         <v>12</v>
       </c>
       <c r="V38">
-        <f>(S38-1)*4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="W38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1701,6 +1921,3727 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296D7A3E-D33F-49E4-A212-60F607EA8E1E}">
+  <dimension ref="A1:AB266"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>TEXT(DATE(2023,7,20),"dd-mmm-yyyy")</f>
+        <v>20-Jul-2023</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I16" cm="1">
+        <f t="array" ref="I16:J16">_xlfn.SEQUENCE(,2,0,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" t="str" cm="1">
+        <f t="array" ref="C18:D20">SplitCols(_tTest[],1,2)</f>
+        <v>A</v>
+      </c>
+      <c r="D18" t="str">
+        <v>B</v>
+      </c>
+      <c r="L18" cm="1">
+        <f t="array" ref="L18:Q18">_xlfn.SEQUENCE(,COLUMNS(_tTest[])/2,1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>9</v>
+      </c>
+      <c r="Q18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C19" t="str">
+        <v>G</v>
+      </c>
+      <c r="D19" t="str">
+        <v>H</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C20" t="str">
+        <v>M</v>
+      </c>
+      <c r="D20" t="str">
+        <v>N</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23" t="str" cm="1">
+        <f t="array" ref="C23:D31">_xlfn.VSTACK(SplitCols(_tTest[],1,2),SplitCols(_tTest[],3,4),SplitCols(_tTest[],5,6))</f>
+        <v>A</v>
+      </c>
+      <c r="D23" t="str">
+        <v>B</v>
+      </c>
+      <c r="F23" t="str" cm="1">
+        <f t="array" ref="F23:G31">_xlfn.DROP(_xlfn.REDUCE({0,0},{1,3,5},_xlfn.LAMBDA(_xlpm.x,_xlpm.y, _xlfn.VSTACK(_xlpm.x,SplitCols(_tTest[],_xlpm.y,_xlpm.y+1)))),1)</f>
+        <v>A</v>
+      </c>
+      <c r="G23" t="str">
+        <v>B</v>
+      </c>
+      <c r="I23" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="I23" ca="1">_xlfn.DROP(_xlfn.REDUCE(_xlfn.SEQUENCE(,2,0,0),_xlfn.SEQUENCE(,COLUMNS(_tTest[])/2,1,2),_xlfn.LAMBDA(_xlpm.x,_xlpm.y, _xlfn.VSTACK(_xlpm.x,SplitCols(_tTest[],_xlpm.y,_xlpm.y+1)))),1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" t="str">
+        <v>G</v>
+      </c>
+      <c r="D24" t="str">
+        <v>H</v>
+      </c>
+      <c r="F24" t="str">
+        <v>G</v>
+      </c>
+      <c r="G24" t="str">
+        <v>H</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" t="str">
+        <v>M</v>
+      </c>
+      <c r="D25" t="str">
+        <v>N</v>
+      </c>
+      <c r="F25" t="str">
+        <v>M</v>
+      </c>
+      <c r="G25" t="str">
+        <v>N</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" t="str">
+        <v>C</v>
+      </c>
+      <c r="D26" t="str">
+        <v>D</v>
+      </c>
+      <c r="F26" t="str">
+        <v>C</v>
+      </c>
+      <c r="G26" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27" t="str">
+        <v>I</v>
+      </c>
+      <c r="D27" t="str">
+        <v>J</v>
+      </c>
+      <c r="F27" t="str">
+        <v>I</v>
+      </c>
+      <c r="G27" t="str">
+        <v>J</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" t="str">
+        <v>O</v>
+      </c>
+      <c r="D28" t="str">
+        <v>P</v>
+      </c>
+      <c r="F28" t="str">
+        <v>O</v>
+      </c>
+      <c r="G28" t="str">
+        <v>P</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" t="str">
+        <v>E</v>
+      </c>
+      <c r="D29" t="str">
+        <v>F</v>
+      </c>
+      <c r="F29" t="str">
+        <v>E</v>
+      </c>
+      <c r="G29" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <v>K</v>
+      </c>
+      <c r="D30" t="str">
+        <v>L</v>
+      </c>
+      <c r="F30" t="str">
+        <v>K</v>
+      </c>
+      <c r="G30" t="str">
+        <v>L</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" t="str">
+        <v>Q</v>
+      </c>
+      <c r="D31" t="str">
+        <v>R</v>
+      </c>
+      <c r="F31" t="str">
+        <v>Q</v>
+      </c>
+      <c r="G31" t="str">
+        <v>R</v>
+      </c>
+    </row>
+    <row r="34" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I34" t="str" cm="1">
+        <f t="array" ref="I34:J51">_xlfn.LAMBDA(_xlpm.array,
+   _xlfn.DROP(
+     _xlfn.REDUCE(
+       {0,0},
+       _xlfn.SEQUENCE(
+         ,
+         COLUMNS(
+           _xlpm.array)/2,1,2),
+       _xlfn.LAMBDA(_xlpm.x,_xlpm.y,
+         _xlfn.VSTACK(
+           _xlpm.x,
+           SplitCols(
+             _xlpm.array,_xlpm.y,_xlpm.y+1)))),1))(_tTest[])</f>
+        <v>A</v>
+      </c>
+      <c r="J34" t="str">
+        <v>B</v>
+      </c>
+      <c r="L34" t="str" cm="1">
+        <f t="array" ref="L34:M51">Stacker(_tTest[])</f>
+        <v>A</v>
+      </c>
+      <c r="M34" t="str">
+        <v>B</v>
+      </c>
+      <c r="Q34" t="str" cm="1">
+        <f t="array" ref="Q34:R51">_xlfn.LAMBDA(_xlpm.array,_xlpm.cols,
+   _xlfn.DROP(
+     _xlfn.REDUCE(
+       _xlfn.SEQUENCE(,_xlpm.cols,0,0),
+       _xlfn.SEQUENCE(
+         ,
+         COLUMNS(
+           _xlpm.array)/_xlpm.cols,1,_xlpm.cols),
+       _xlfn.LAMBDA(_xlpm.x,_xlpm.y,
+         _xlfn.VSTACK(
+           _xlpm.x,
+           SplitCols(
+             _xlpm.array,_xlpm.y,_xlpm.y+_xlpm.cols-1)))),1))(_tTest[],2)</f>
+        <v>A</v>
+      </c>
+      <c r="R34" t="str">
+        <v>B</v>
+      </c>
+      <c r="X34" t="str" cm="1">
+        <f t="array" ref="X34:AB39">Stacker2(_tTest[],5)</f>
+        <v>A</v>
+      </c>
+      <c r="Y34" t="str">
+        <v>B</v>
+      </c>
+      <c r="Z34" t="str">
+        <v>C</v>
+      </c>
+      <c r="AA34" t="str">
+        <v>D</v>
+      </c>
+      <c r="AB34" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="35" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I35" t="str">
+        <v>G</v>
+      </c>
+      <c r="J35" t="str">
+        <v>H</v>
+      </c>
+      <c r="L35" t="str">
+        <v>G</v>
+      </c>
+      <c r="M35" t="str">
+        <v>H</v>
+      </c>
+      <c r="Q35" t="str">
+        <v>G</v>
+      </c>
+      <c r="R35" t="str">
+        <v>H</v>
+      </c>
+      <c r="X35" t="str">
+        <v>G</v>
+      </c>
+      <c r="Y35" t="str">
+        <v>H</v>
+      </c>
+      <c r="Z35" t="str">
+        <v>I</v>
+      </c>
+      <c r="AA35" t="str">
+        <v>J</v>
+      </c>
+      <c r="AB35" t="str">
+        <v>K</v>
+      </c>
+    </row>
+    <row r="36" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I36" t="str">
+        <v>M</v>
+      </c>
+      <c r="J36" t="str">
+        <v>N</v>
+      </c>
+      <c r="L36" t="str">
+        <v>M</v>
+      </c>
+      <c r="M36" t="str">
+        <v>N</v>
+      </c>
+      <c r="Q36" t="str">
+        <v>M</v>
+      </c>
+      <c r="R36" t="str">
+        <v>N</v>
+      </c>
+      <c r="X36" t="str">
+        <v>M</v>
+      </c>
+      <c r="Y36" t="str">
+        <v>N</v>
+      </c>
+      <c r="Z36" t="str">
+        <v>O</v>
+      </c>
+      <c r="AA36" t="str">
+        <v>P</v>
+      </c>
+      <c r="AB36" t="str">
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="37" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I37" t="str">
+        <v>C</v>
+      </c>
+      <c r="J37" t="str">
+        <v>D</v>
+      </c>
+      <c r="L37" t="str">
+        <v>C</v>
+      </c>
+      <c r="M37" t="str">
+        <v>D</v>
+      </c>
+      <c r="Q37" t="str">
+        <v>C</v>
+      </c>
+      <c r="R37" t="str">
+        <v>D</v>
+      </c>
+      <c r="X37" t="str">
+        <v>F</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
+      <c r="Z37">
+        <v>4</v>
+      </c>
+      <c r="AA37" t="str">
+        <v>aa</v>
+      </c>
+      <c r="AB37" t="str">
+        <v>ad</v>
+      </c>
+    </row>
+    <row r="38" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I38" t="str">
+        <v>I</v>
+      </c>
+      <c r="J38" t="str">
+        <v>J</v>
+      </c>
+      <c r="L38" t="str">
+        <v>I</v>
+      </c>
+      <c r="M38" t="str">
+        <v>J</v>
+      </c>
+      <c r="Q38" t="str">
+        <v>I</v>
+      </c>
+      <c r="R38" t="str">
+        <v>J</v>
+      </c>
+      <c r="X38" t="str">
+        <v>L</v>
+      </c>
+      <c r="Y38">
+        <v>2</v>
+      </c>
+      <c r="Z38">
+        <v>5</v>
+      </c>
+      <c r="AA38" t="str">
+        <v>ab</v>
+      </c>
+      <c r="AB38" t="str">
+        <v>ae</v>
+      </c>
+    </row>
+    <row r="39" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I39" t="str">
+        <v>O</v>
+      </c>
+      <c r="J39" t="str">
+        <v>P</v>
+      </c>
+      <c r="L39" t="str">
+        <v>O</v>
+      </c>
+      <c r="M39" t="str">
+        <v>P</v>
+      </c>
+      <c r="Q39" t="str">
+        <v>O</v>
+      </c>
+      <c r="R39" t="str">
+        <v>P</v>
+      </c>
+      <c r="X39" t="str">
+        <v>R</v>
+      </c>
+      <c r="Y39">
+        <v>3</v>
+      </c>
+      <c r="Z39">
+        <v>6</v>
+      </c>
+      <c r="AA39" t="str">
+        <v>ac</v>
+      </c>
+      <c r="AB39" t="str">
+        <v>af</v>
+      </c>
+    </row>
+    <row r="40" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I40" t="str">
+        <v>E</v>
+      </c>
+      <c r="J40" t="str">
+        <v>F</v>
+      </c>
+      <c r="L40" t="str">
+        <v>E</v>
+      </c>
+      <c r="M40" t="str">
+        <v>F</v>
+      </c>
+      <c r="Q40" t="str">
+        <v>E</v>
+      </c>
+      <c r="R40" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="41" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I41" t="str">
+        <v>K</v>
+      </c>
+      <c r="J41" t="str">
+        <v>L</v>
+      </c>
+      <c r="L41" t="str">
+        <v>K</v>
+      </c>
+      <c r="M41" t="str">
+        <v>L</v>
+      </c>
+      <c r="Q41" t="str">
+        <v>K</v>
+      </c>
+      <c r="R41" t="str">
+        <v>L</v>
+      </c>
+    </row>
+    <row r="42" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I42" t="str">
+        <v>Q</v>
+      </c>
+      <c r="J42" t="str">
+        <v>R</v>
+      </c>
+      <c r="L42" t="str">
+        <v>Q</v>
+      </c>
+      <c r="M42" t="str">
+        <v>R</v>
+      </c>
+      <c r="Q42" t="str">
+        <v>Q</v>
+      </c>
+      <c r="R42" t="str">
+        <v>R</v>
+      </c>
+    </row>
+    <row r="43" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>4</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>5</v>
+      </c>
+      <c r="L44">
+        <v>2</v>
+      </c>
+      <c r="M44">
+        <v>5</v>
+      </c>
+      <c r="Q44">
+        <v>2</v>
+      </c>
+      <c r="R44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="L45">
+        <v>3</v>
+      </c>
+      <c r="M45">
+        <v>6</v>
+      </c>
+      <c r="Q45">
+        <v>3</v>
+      </c>
+      <c r="R45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I46" t="str">
+        <v>aa</v>
+      </c>
+      <c r="J46" t="str">
+        <v>ad</v>
+      </c>
+      <c r="L46" t="str">
+        <v>aa</v>
+      </c>
+      <c r="M46" t="str">
+        <v>ad</v>
+      </c>
+      <c r="Q46" t="str">
+        <v>aa</v>
+      </c>
+      <c r="R46" t="str">
+        <v>ad</v>
+      </c>
+    </row>
+    <row r="47" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I47" t="str">
+        <v>ab</v>
+      </c>
+      <c r="J47" t="str">
+        <v>ae</v>
+      </c>
+      <c r="L47" t="str">
+        <v>ab</v>
+      </c>
+      <c r="M47" t="str">
+        <v>ae</v>
+      </c>
+      <c r="Q47" t="str">
+        <v>ab</v>
+      </c>
+      <c r="R47" t="str">
+        <v>ae</v>
+      </c>
+    </row>
+    <row r="48" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I48" t="str">
+        <v>ac</v>
+      </c>
+      <c r="J48" t="str">
+        <v>af</v>
+      </c>
+      <c r="L48" t="str">
+        <v>ac</v>
+      </c>
+      <c r="M48" t="str">
+        <v>af</v>
+      </c>
+      <c r="Q48" t="str">
+        <v>ac</v>
+      </c>
+      <c r="R48" t="str">
+        <v>af</v>
+      </c>
+    </row>
+    <row r="49" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="I49" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J49" t="str">
+        <v>yy</v>
+      </c>
+      <c r="L49" t="str">
+        <v>zz</v>
+      </c>
+      <c r="M49" t="str">
+        <v>yy</v>
+      </c>
+      <c r="Q49" t="str">
+        <v>zz</v>
+      </c>
+      <c r="R49" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="50" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="I50" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J50" t="str">
+        <v>yy</v>
+      </c>
+      <c r="L50" t="str">
+        <v>zz</v>
+      </c>
+      <c r="M50" t="str">
+        <v>yy</v>
+      </c>
+      <c r="Q50" t="str">
+        <v>zz</v>
+      </c>
+      <c r="R50" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="51" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="I51" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J51" t="str">
+        <v>yy</v>
+      </c>
+      <c r="L51" t="str">
+        <v>zz</v>
+      </c>
+      <c r="M51" t="str">
+        <v>yy</v>
+      </c>
+      <c r="Q51" t="str">
+        <v>zz</v>
+      </c>
+      <c r="R51" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="61" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>3.0822630000000002</v>
+      </c>
+      <c r="G61">
+        <v>25</v>
+      </c>
+      <c r="H61">
+        <v>3.6292970000000002</v>
+      </c>
+      <c r="I61">
+        <v>50</v>
+      </c>
+      <c r="J61">
+        <v>3.7472940000000001</v>
+      </c>
+      <c r="K61">
+        <v>75</v>
+      </c>
+      <c r="L61">
+        <v>3.9751690000000002</v>
+      </c>
+      <c r="P61" cm="1">
+        <f t="array" ref="P61:Q160">Stacker2(E61:L85,2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>3.0822630000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>3.2301890000000002</v>
+      </c>
+      <c r="G62">
+        <v>26</v>
+      </c>
+      <c r="H62">
+        <v>3.6335190000000002</v>
+      </c>
+      <c r="I62">
+        <v>51</v>
+      </c>
+      <c r="J62">
+        <v>3.7538320000000001</v>
+      </c>
+      <c r="K62">
+        <v>76</v>
+      </c>
+      <c r="L62">
+        <v>3.9859170000000002</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>3.2301890000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>3.3168229999999999</v>
+      </c>
+      <c r="G63">
+        <v>27</v>
+      </c>
+      <c r="H63">
+        <v>3.637324</v>
+      </c>
+      <c r="I63">
+        <v>52</v>
+      </c>
+      <c r="J63">
+        <v>3.7604199999999999</v>
+      </c>
+      <c r="K63">
+        <v>77</v>
+      </c>
+      <c r="L63">
+        <v>3.9967329999999999</v>
+      </c>
+      <c r="P63">
+        <v>2</v>
+      </c>
+      <c r="Q63">
+        <v>3.3168229999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>3.3811659999999999</v>
+      </c>
+      <c r="G64">
+        <v>28</v>
+      </c>
+      <c r="H64">
+        <v>3.6413039999999999</v>
+      </c>
+      <c r="I64">
+        <v>53</v>
+      </c>
+      <c r="J64">
+        <v>3.7674280000000002</v>
+      </c>
+      <c r="K64">
+        <v>78</v>
+      </c>
+      <c r="L64">
+        <v>4.0076650000000003</v>
+      </c>
+      <c r="P64">
+        <v>3</v>
+      </c>
+      <c r="Q64">
+        <v>3.3811659999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>3.4311829999999999</v>
+      </c>
+      <c r="G65">
+        <v>29</v>
+      </c>
+      <c r="H65">
+        <v>3.64567</v>
+      </c>
+      <c r="I65">
+        <v>54</v>
+      </c>
+      <c r="J65">
+        <v>3.774896</v>
+      </c>
+      <c r="K65">
+        <v>79</v>
+      </c>
+      <c r="L65">
+        <v>4.0185440000000003</v>
+      </c>
+      <c r="P65">
+        <v>4</v>
+      </c>
+      <c r="Q65">
+        <v>3.4311829999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66">
+        <v>3.4698280000000001</v>
+      </c>
+      <c r="G66">
+        <v>30</v>
+      </c>
+      <c r="H66">
+        <v>3.6493099999999998</v>
+      </c>
+      <c r="I66">
+        <v>55</v>
+      </c>
+      <c r="J66">
+        <v>3.7825730000000002</v>
+      </c>
+      <c r="K66">
+        <v>80</v>
+      </c>
+      <c r="L66">
+        <v>4.0295370000000004</v>
+      </c>
+      <c r="P66">
+        <v>5</v>
+      </c>
+      <c r="Q66">
+        <v>3.4698280000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>6</v>
+      </c>
+      <c r="F67">
+        <v>3.4855589999999999</v>
+      </c>
+      <c r="G67">
+        <v>31</v>
+      </c>
+      <c r="H67">
+        <v>3.6531560000000001</v>
+      </c>
+      <c r="I67">
+        <v>56</v>
+      </c>
+      <c r="J67">
+        <v>3.7906659999999999</v>
+      </c>
+      <c r="K67">
+        <v>81</v>
+      </c>
+      <c r="L67">
+        <v>4.041086</v>
+      </c>
+      <c r="P67">
+        <v>6</v>
+      </c>
+      <c r="Q67">
+        <v>3.4855589999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>7</v>
+      </c>
+      <c r="F68">
+        <v>3.4923329999999999</v>
+      </c>
+      <c r="G68">
+        <v>32</v>
+      </c>
+      <c r="H68">
+        <v>3.6569940000000001</v>
+      </c>
+      <c r="I68">
+        <v>57</v>
+      </c>
+      <c r="J68">
+        <v>3.7990330000000001</v>
+      </c>
+      <c r="K68">
+        <v>82</v>
+      </c>
+      <c r="L68">
+        <v>4.0520930000000002</v>
+      </c>
+      <c r="P68">
+        <v>7</v>
+      </c>
+      <c r="Q68">
+        <v>3.4923329999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>8</v>
+      </c>
+      <c r="F69">
+        <v>3.4986649999999999</v>
+      </c>
+      <c r="G69">
+        <v>33</v>
+      </c>
+      <c r="H69">
+        <v>3.661524</v>
+      </c>
+      <c r="I69">
+        <v>58</v>
+      </c>
+      <c r="J69">
+        <v>3.8074910000000002</v>
+      </c>
+      <c r="K69">
+        <v>83</v>
+      </c>
+      <c r="L69">
+        <v>4.063879</v>
+      </c>
+      <c r="P69">
+        <v>8</v>
+      </c>
+      <c r="Q69">
+        <v>3.4986649999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>9</v>
+      </c>
+      <c r="F70">
+        <v>3.5051670000000001</v>
+      </c>
+      <c r="G70">
+        <v>34</v>
+      </c>
+      <c r="H70">
+        <v>3.6656279999999999</v>
+      </c>
+      <c r="I70">
+        <v>59</v>
+      </c>
+      <c r="J70">
+        <v>3.8157480000000001</v>
+      </c>
+      <c r="K70">
+        <v>84</v>
+      </c>
+      <c r="L70">
+        <v>4.075736</v>
+      </c>
+      <c r="P70">
+        <v>9</v>
+      </c>
+      <c r="Q70">
+        <v>3.5051670000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>10</v>
+      </c>
+      <c r="F71">
+        <v>3.5121000000000002</v>
+      </c>
+      <c r="G71">
+        <v>35</v>
+      </c>
+      <c r="H71">
+        <v>3.6697329999999999</v>
+      </c>
+      <c r="I71">
+        <v>60</v>
+      </c>
+      <c r="J71">
+        <v>3.8251330000000001</v>
+      </c>
+      <c r="K71">
+        <v>85</v>
+      </c>
+      <c r="L71">
+        <v>4.0872869999999999</v>
+      </c>
+      <c r="P71">
+        <v>10</v>
+      </c>
+      <c r="Q71">
+        <v>3.5121000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>11</v>
+      </c>
+      <c r="F72">
+        <v>3.518983</v>
+      </c>
+      <c r="G72">
+        <v>36</v>
+      </c>
+      <c r="H72">
+        <v>3.6741440000000001</v>
+      </c>
+      <c r="I72">
+        <v>61</v>
+      </c>
+      <c r="J72">
+        <v>3.8339430000000001</v>
+      </c>
+      <c r="K72">
+        <v>86</v>
+      </c>
+      <c r="L72">
+        <v>4.0992829999999998</v>
+      </c>
+      <c r="P72">
+        <v>11</v>
+      </c>
+      <c r="Q72">
+        <v>3.518983</v>
+      </c>
+    </row>
+    <row r="73" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>12</v>
+      </c>
+      <c r="F73">
+        <v>3.5258820000000002</v>
+      </c>
+      <c r="G73">
+        <v>37</v>
+      </c>
+      <c r="H73">
+        <v>3.6783809999999999</v>
+      </c>
+      <c r="I73">
+        <v>62</v>
+      </c>
+      <c r="J73">
+        <v>3.8435790000000001</v>
+      </c>
+      <c r="K73">
+        <v>87</v>
+      </c>
+      <c r="L73">
+        <v>4.1116109999999999</v>
+      </c>
+      <c r="P73">
+        <v>12</v>
+      </c>
+      <c r="Q73">
+        <v>3.5258820000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>13</v>
+      </c>
+      <c r="F74">
+        <v>3.533115</v>
+      </c>
+      <c r="G74">
+        <v>38</v>
+      </c>
+      <c r="H74">
+        <v>3.6827390000000002</v>
+      </c>
+      <c r="I74">
+        <v>63</v>
+      </c>
+      <c r="J74">
+        <v>3.8529080000000002</v>
+      </c>
+      <c r="K74">
+        <v>88</v>
+      </c>
+      <c r="L74">
+        <v>4.1237729999999999</v>
+      </c>
+      <c r="P74">
+        <v>13</v>
+      </c>
+      <c r="Q74">
+        <v>3.533115</v>
+      </c>
+    </row>
+    <row r="75" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>14</v>
+      </c>
+      <c r="F75">
+        <v>3.541426</v>
+      </c>
+      <c r="G75">
+        <v>39</v>
+      </c>
+      <c r="H75">
+        <v>3.6873710000000002</v>
+      </c>
+      <c r="I75">
+        <v>64</v>
+      </c>
+      <c r="J75">
+        <v>3.8626680000000002</v>
+      </c>
+      <c r="K75">
+        <v>89</v>
+      </c>
+      <c r="L75">
+        <v>4.1360049999999999</v>
+      </c>
+      <c r="P75">
+        <v>14</v>
+      </c>
+      <c r="Q75">
+        <v>3.541426</v>
+      </c>
+    </row>
+    <row r="76" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>15</v>
+      </c>
+      <c r="F76">
+        <v>3.5503450000000001</v>
+      </c>
+      <c r="G76">
+        <v>40</v>
+      </c>
+      <c r="H76">
+        <v>3.6918000000000002</v>
+      </c>
+      <c r="I76">
+        <v>65</v>
+      </c>
+      <c r="J76">
+        <v>3.8725390000000002</v>
+      </c>
+      <c r="K76">
+        <v>90</v>
+      </c>
+      <c r="L76">
+        <v>4.1484990000000002</v>
+      </c>
+      <c r="P76">
+        <v>15</v>
+      </c>
+      <c r="Q76">
+        <v>3.5503450000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>16</v>
+      </c>
+      <c r="F77">
+        <v>3.5596830000000002</v>
+      </c>
+      <c r="G77">
+        <v>41</v>
+      </c>
+      <c r="H77">
+        <v>3.6964260000000002</v>
+      </c>
+      <c r="I77">
+        <v>66</v>
+      </c>
+      <c r="J77">
+        <v>3.8825910000000001</v>
+      </c>
+      <c r="K77">
+        <v>91</v>
+      </c>
+      <c r="L77">
+        <v>4.1610300000000002</v>
+      </c>
+      <c r="P77">
+        <v>16</v>
+      </c>
+      <c r="Q77">
+        <v>3.5596830000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>17</v>
+      </c>
+      <c r="F78">
+        <v>3.5688110000000002</v>
+      </c>
+      <c r="G78">
+        <v>42</v>
+      </c>
+      <c r="H78">
+        <v>3.7016909999999998</v>
+      </c>
+      <c r="I78">
+        <v>67</v>
+      </c>
+      <c r="J78">
+        <v>3.8923559999999999</v>
+      </c>
+      <c r="K78">
+        <v>92</v>
+      </c>
+      <c r="L78">
+        <v>4.1737729999999997</v>
+      </c>
+      <c r="P78">
+        <v>17</v>
+      </c>
+      <c r="Q78">
+        <v>3.5688110000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>18</v>
+      </c>
+      <c r="F79">
+        <v>3.5781299999999998</v>
+      </c>
+      <c r="G79">
+        <v>43</v>
+      </c>
+      <c r="H79">
+        <v>3.7068789999999998</v>
+      </c>
+      <c r="I79">
+        <v>68</v>
+      </c>
+      <c r="J79">
+        <v>3.9026320000000001</v>
+      </c>
+      <c r="K79">
+        <v>93</v>
+      </c>
+      <c r="L79">
+        <v>4.1867080000000003</v>
+      </c>
+      <c r="P79">
+        <v>18</v>
+      </c>
+      <c r="Q79">
+        <v>3.5781299999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>19</v>
+      </c>
+      <c r="F80">
+        <v>3.5870760000000002</v>
+      </c>
+      <c r="G80">
+        <v>44</v>
+      </c>
+      <c r="H80">
+        <v>3.7122130000000002</v>
+      </c>
+      <c r="I80">
+        <v>69</v>
+      </c>
+      <c r="J80">
+        <v>3.9126699999999999</v>
+      </c>
+      <c r="K80">
+        <v>94</v>
+      </c>
+      <c r="L80">
+        <v>4.1996310000000001</v>
+      </c>
+      <c r="P80">
+        <v>19</v>
+      </c>
+      <c r="Q80">
+        <v>3.5870760000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>20</v>
+      </c>
+      <c r="F81">
+        <v>3.5958990000000002</v>
+      </c>
+      <c r="G81">
+        <v>45</v>
+      </c>
+      <c r="H81">
+        <v>3.7175470000000002</v>
+      </c>
+      <c r="I81">
+        <v>70</v>
+      </c>
+      <c r="J81">
+        <v>3.9228160000000001</v>
+      </c>
+      <c r="K81">
+        <v>95</v>
+      </c>
+      <c r="L81">
+        <v>4.2</v>
+      </c>
+      <c r="P81">
+        <v>20</v>
+      </c>
+      <c r="Q81">
+        <v>3.5958990000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>21</v>
+      </c>
+      <c r="F82">
+        <v>3.6044960000000001</v>
+      </c>
+      <c r="G82">
+        <v>46</v>
+      </c>
+      <c r="H82">
+        <v>3.7231869999999998</v>
+      </c>
+      <c r="I82">
+        <v>71</v>
+      </c>
+      <c r="J82">
+        <v>3.9329779999999999</v>
+      </c>
+      <c r="K82">
+        <v>96</v>
+      </c>
+      <c r="L82">
+        <v>4.2</v>
+      </c>
+      <c r="P82">
+        <v>21</v>
+      </c>
+      <c r="Q82">
+        <v>3.6044960000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>22</v>
+      </c>
+      <c r="F83">
+        <v>3.6123430000000001</v>
+      </c>
+      <c r="G83">
+        <v>47</v>
+      </c>
+      <c r="H83">
+        <v>3.729136</v>
+      </c>
+      <c r="I83">
+        <v>72</v>
+      </c>
+      <c r="J83">
+        <v>3.9435959999999999</v>
+      </c>
+      <c r="K83">
+        <v>97</v>
+      </c>
+      <c r="L83">
+        <v>4.2</v>
+      </c>
+      <c r="P83">
+        <v>22</v>
+      </c>
+      <c r="Q83">
+        <v>3.6123430000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>23</v>
+      </c>
+      <c r="F84">
+        <v>3.618935</v>
+      </c>
+      <c r="G84">
+        <v>48</v>
+      </c>
+      <c r="H84">
+        <v>3.735087</v>
+      </c>
+      <c r="I84">
+        <v>73</v>
+      </c>
+      <c r="J84">
+        <v>3.9539240000000002</v>
+      </c>
+      <c r="K84">
+        <v>98</v>
+      </c>
+      <c r="L84">
+        <v>4.2</v>
+      </c>
+      <c r="P84">
+        <v>23</v>
+      </c>
+      <c r="Q84">
+        <v>3.618935</v>
+      </c>
+    </row>
+    <row r="85" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>24</v>
+      </c>
+      <c r="F85">
+        <v>3.6247229999999999</v>
+      </c>
+      <c r="G85">
+        <v>49</v>
+      </c>
+      <c r="H85">
+        <v>3.7408130000000002</v>
+      </c>
+      <c r="I85">
+        <v>74</v>
+      </c>
+      <c r="J85">
+        <v>3.9642330000000001</v>
+      </c>
+      <c r="K85">
+        <v>99</v>
+      </c>
+      <c r="L85">
+        <v>4.2</v>
+      </c>
+      <c r="P85">
+        <v>24</v>
+      </c>
+      <c r="Q85">
+        <v>3.6247229999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P86">
+        <v>25</v>
+      </c>
+      <c r="Q86">
+        <v>3.6292970000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P87">
+        <v>26</v>
+      </c>
+      <c r="Q87">
+        <v>3.6335190000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P88">
+        <v>27</v>
+      </c>
+      <c r="Q88">
+        <v>3.637324</v>
+      </c>
+    </row>
+    <row r="89" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P89">
+        <v>28</v>
+      </c>
+      <c r="Q89">
+        <v>3.6413039999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P90">
+        <v>29</v>
+      </c>
+      <c r="Q90">
+        <v>3.64567</v>
+      </c>
+    </row>
+    <row r="91" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P91">
+        <v>30</v>
+      </c>
+      <c r="Q91">
+        <v>3.6493099999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>100</v>
+      </c>
+      <c r="F92">
+        <v>4.2</v>
+      </c>
+      <c r="P92">
+        <v>31</v>
+      </c>
+      <c r="Q92">
+        <v>3.6531560000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P93">
+        <v>32</v>
+      </c>
+      <c r="Q93">
+        <v>3.6569940000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P94">
+        <v>33</v>
+      </c>
+      <c r="Q94">
+        <v>3.661524</v>
+      </c>
+    </row>
+    <row r="95" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P95">
+        <v>34</v>
+      </c>
+      <c r="Q95">
+        <v>3.6656279999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P96">
+        <v>35</v>
+      </c>
+      <c r="Q96">
+        <v>3.6697329999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P97">
+        <v>36</v>
+      </c>
+      <c r="Q97">
+        <v>3.6741440000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P98">
+        <v>37</v>
+      </c>
+      <c r="Q98">
+        <v>3.6783809999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P99">
+        <v>38</v>
+      </c>
+      <c r="Q99">
+        <v>3.6827390000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P100">
+        <v>39</v>
+      </c>
+      <c r="Q100">
+        <v>3.6873710000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P101">
+        <v>40</v>
+      </c>
+      <c r="Q101">
+        <v>3.6918000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P102">
+        <v>41</v>
+      </c>
+      <c r="Q102">
+        <v>3.6964260000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P103">
+        <v>42</v>
+      </c>
+      <c r="Q103">
+        <v>3.7016909999999998</v>
+      </c>
+    </row>
+    <row r="104" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P104">
+        <v>43</v>
+      </c>
+      <c r="Q104">
+        <v>3.7068789999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P105">
+        <v>44</v>
+      </c>
+      <c r="Q105">
+        <v>3.7122130000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P106">
+        <v>45</v>
+      </c>
+      <c r="Q106">
+        <v>3.7175470000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P107">
+        <v>46</v>
+      </c>
+      <c r="Q107">
+        <v>3.7231869999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P108">
+        <v>47</v>
+      </c>
+      <c r="Q108">
+        <v>3.729136</v>
+      </c>
+    </row>
+    <row r="109" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P109">
+        <v>48</v>
+      </c>
+      <c r="Q109">
+        <v>3.735087</v>
+      </c>
+    </row>
+    <row r="110" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P110">
+        <v>49</v>
+      </c>
+      <c r="Q110">
+        <v>3.7408130000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P111">
+        <v>50</v>
+      </c>
+      <c r="Q111">
+        <v>3.7472940000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P112">
+        <v>51</v>
+      </c>
+      <c r="Q112">
+        <v>3.7538320000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P113">
+        <v>52</v>
+      </c>
+      <c r="Q113">
+        <v>3.7604199999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P114">
+        <v>53</v>
+      </c>
+      <c r="Q114">
+        <v>3.7674280000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P115">
+        <v>54</v>
+      </c>
+      <c r="Q115">
+        <v>3.774896</v>
+      </c>
+    </row>
+    <row r="116" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P116">
+        <v>55</v>
+      </c>
+      <c r="Q116">
+        <v>3.7825730000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P117">
+        <v>56</v>
+      </c>
+      <c r="Q117">
+        <v>3.7906659999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P118">
+        <v>57</v>
+      </c>
+      <c r="Q118">
+        <v>3.7990330000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P119">
+        <v>58</v>
+      </c>
+      <c r="Q119">
+        <v>3.8074910000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P120">
+        <v>59</v>
+      </c>
+      <c r="Q120">
+        <v>3.8157480000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P121">
+        <v>60</v>
+      </c>
+      <c r="Q121">
+        <v>3.8251330000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P122">
+        <v>61</v>
+      </c>
+      <c r="Q122">
+        <v>3.8339430000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P123">
+        <v>62</v>
+      </c>
+      <c r="Q123">
+        <v>3.8435790000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P124">
+        <v>63</v>
+      </c>
+      <c r="Q124">
+        <v>3.8529080000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P125">
+        <v>64</v>
+      </c>
+      <c r="Q125">
+        <v>3.8626680000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P126">
+        <v>65</v>
+      </c>
+      <c r="Q126">
+        <v>3.8725390000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P127">
+        <v>66</v>
+      </c>
+      <c r="Q127">
+        <v>3.8825910000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P128">
+        <v>67</v>
+      </c>
+      <c r="Q128">
+        <v>3.8923559999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P129">
+        <v>68</v>
+      </c>
+      <c r="Q129">
+        <v>3.9026320000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P130">
+        <v>69</v>
+      </c>
+      <c r="Q130">
+        <v>3.9126699999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P131">
+        <v>70</v>
+      </c>
+      <c r="Q131">
+        <v>3.9228160000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P132">
+        <v>71</v>
+      </c>
+      <c r="Q132">
+        <v>3.9329779999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P133">
+        <v>72</v>
+      </c>
+      <c r="Q133">
+        <v>3.9435959999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P134">
+        <v>73</v>
+      </c>
+      <c r="Q134">
+        <v>3.9539240000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P135">
+        <v>74</v>
+      </c>
+      <c r="Q135">
+        <v>3.9642330000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P136">
+        <v>75</v>
+      </c>
+      <c r="Q136">
+        <v>3.9751690000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P137">
+        <v>76</v>
+      </c>
+      <c r="Q137">
+        <v>3.9859170000000002</v>
+      </c>
+    </row>
+    <row r="138" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P138">
+        <v>77</v>
+      </c>
+      <c r="Q138">
+        <v>3.9967329999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P139">
+        <v>78</v>
+      </c>
+      <c r="Q139">
+        <v>4.0076650000000003</v>
+      </c>
+    </row>
+    <row r="140" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P140">
+        <v>79</v>
+      </c>
+      <c r="Q140">
+        <v>4.0185440000000003</v>
+      </c>
+    </row>
+    <row r="141" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P141">
+        <v>80</v>
+      </c>
+      <c r="Q141">
+        <v>4.0295370000000004</v>
+      </c>
+    </row>
+    <row r="142" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P142">
+        <v>81</v>
+      </c>
+      <c r="Q142">
+        <v>4.041086</v>
+      </c>
+    </row>
+    <row r="143" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P143">
+        <v>82</v>
+      </c>
+      <c r="Q143">
+        <v>4.0520930000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P144">
+        <v>83</v>
+      </c>
+      <c r="Q144">
+        <v>4.063879</v>
+      </c>
+    </row>
+    <row r="145" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P145">
+        <v>84</v>
+      </c>
+      <c r="Q145">
+        <v>4.075736</v>
+      </c>
+    </row>
+    <row r="146" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P146">
+        <v>85</v>
+      </c>
+      <c r="Q146">
+        <v>4.0872869999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P147">
+        <v>86</v>
+      </c>
+      <c r="Q147">
+        <v>4.0992829999999998</v>
+      </c>
+    </row>
+    <row r="148" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P148">
+        <v>87</v>
+      </c>
+      <c r="Q148">
+        <v>4.1116109999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P149">
+        <v>88</v>
+      </c>
+      <c r="Q149">
+        <v>4.1237729999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P150">
+        <v>89</v>
+      </c>
+      <c r="Q150">
+        <v>4.1360049999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P151">
+        <v>90</v>
+      </c>
+      <c r="Q151">
+        <v>4.1484990000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P152">
+        <v>91</v>
+      </c>
+      <c r="Q152">
+        <v>4.1610300000000002</v>
+      </c>
+    </row>
+    <row r="153" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P153">
+        <v>92</v>
+      </c>
+      <c r="Q153">
+        <v>4.1737729999999997</v>
+      </c>
+    </row>
+    <row r="154" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P154">
+        <v>93</v>
+      </c>
+      <c r="Q154">
+        <v>4.1867080000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P155">
+        <v>94</v>
+      </c>
+      <c r="Q155">
+        <v>4.1996310000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P156">
+        <v>95</v>
+      </c>
+      <c r="Q156">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="157" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P157">
+        <v>96</v>
+      </c>
+      <c r="Q157">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="158" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P158">
+        <v>97</v>
+      </c>
+      <c r="Q158">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="159" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P159">
+        <v>98</v>
+      </c>
+      <c r="Q159">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="160" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P160">
+        <v>99</v>
+      </c>
+      <c r="Q160">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="163" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>3.0822630000000002</v>
+      </c>
+      <c r="F163">
+        <v>25</v>
+      </c>
+      <c r="G163">
+        <v>3.6292970000000002</v>
+      </c>
+      <c r="H163">
+        <v>50</v>
+      </c>
+      <c r="I163">
+        <v>3.7472940000000001</v>
+      </c>
+      <c r="J163">
+        <v>75</v>
+      </c>
+      <c r="K163">
+        <v>3.9751690000000002</v>
+      </c>
+      <c r="P163" cm="1">
+        <f t="array" ref="P163:Q266">Stacker2(D163:K188,2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q163">
+        <v>3.0822630000000002</v>
+      </c>
+    </row>
+    <row r="164" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>3.2301890000000002</v>
+      </c>
+      <c r="F164">
+        <v>26</v>
+      </c>
+      <c r="G164">
+        <v>3.6335190000000002</v>
+      </c>
+      <c r="H164">
+        <v>51</v>
+      </c>
+      <c r="I164">
+        <v>3.7538320000000001</v>
+      </c>
+      <c r="J164">
+        <v>76</v>
+      </c>
+      <c r="K164">
+        <v>3.9859170000000002</v>
+      </c>
+      <c r="P164">
+        <v>1</v>
+      </c>
+      <c r="Q164">
+        <v>3.2301890000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165">
+        <v>3.3168229999999999</v>
+      </c>
+      <c r="F165">
+        <v>27</v>
+      </c>
+      <c r="G165">
+        <v>3.637324</v>
+      </c>
+      <c r="H165">
+        <v>52</v>
+      </c>
+      <c r="I165">
+        <v>3.7604199999999999</v>
+      </c>
+      <c r="J165">
+        <v>77</v>
+      </c>
+      <c r="K165">
+        <v>3.9967329999999999</v>
+      </c>
+      <c r="P165">
+        <v>2</v>
+      </c>
+      <c r="Q165">
+        <v>3.3168229999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>3</v>
+      </c>
+      <c r="E166">
+        <v>3.3811659999999999</v>
+      </c>
+      <c r="F166">
+        <v>28</v>
+      </c>
+      <c r="G166">
+        <v>3.6413039999999999</v>
+      </c>
+      <c r="H166">
+        <v>53</v>
+      </c>
+      <c r="I166">
+        <v>3.7674280000000002</v>
+      </c>
+      <c r="J166">
+        <v>78</v>
+      </c>
+      <c r="K166">
+        <v>4.0076650000000003</v>
+      </c>
+      <c r="P166">
+        <v>3</v>
+      </c>
+      <c r="Q166">
+        <v>3.3811659999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D167">
+        <v>4</v>
+      </c>
+      <c r="E167">
+        <v>3.4311829999999999</v>
+      </c>
+      <c r="F167">
+        <v>29</v>
+      </c>
+      <c r="G167">
+        <v>3.64567</v>
+      </c>
+      <c r="H167">
+        <v>54</v>
+      </c>
+      <c r="I167">
+        <v>3.774896</v>
+      </c>
+      <c r="J167">
+        <v>79</v>
+      </c>
+      <c r="K167">
+        <v>4.0185440000000003</v>
+      </c>
+      <c r="P167">
+        <v>4</v>
+      </c>
+      <c r="Q167">
+        <v>3.4311829999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>5</v>
+      </c>
+      <c r="E168">
+        <v>3.4698280000000001</v>
+      </c>
+      <c r="F168">
+        <v>30</v>
+      </c>
+      <c r="G168">
+        <v>3.6493099999999998</v>
+      </c>
+      <c r="H168">
+        <v>55</v>
+      </c>
+      <c r="I168">
+        <v>3.7825730000000002</v>
+      </c>
+      <c r="J168">
+        <v>80</v>
+      </c>
+      <c r="K168">
+        <v>4.0295370000000004</v>
+      </c>
+      <c r="P168">
+        <v>5</v>
+      </c>
+      <c r="Q168">
+        <v>3.4698280000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>6</v>
+      </c>
+      <c r="E169">
+        <v>3.4855589999999999</v>
+      </c>
+      <c r="F169">
+        <v>31</v>
+      </c>
+      <c r="G169">
+        <v>3.6531560000000001</v>
+      </c>
+      <c r="H169">
+        <v>56</v>
+      </c>
+      <c r="I169">
+        <v>3.7906659999999999</v>
+      </c>
+      <c r="J169">
+        <v>81</v>
+      </c>
+      <c r="K169">
+        <v>4.041086</v>
+      </c>
+      <c r="P169">
+        <v>6</v>
+      </c>
+      <c r="Q169">
+        <v>3.4855589999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D170">
+        <v>7</v>
+      </c>
+      <c r="E170">
+        <v>3.4923329999999999</v>
+      </c>
+      <c r="F170">
+        <v>32</v>
+      </c>
+      <c r="G170">
+        <v>3.6569940000000001</v>
+      </c>
+      <c r="H170">
+        <v>57</v>
+      </c>
+      <c r="I170">
+        <v>3.7990330000000001</v>
+      </c>
+      <c r="J170">
+        <v>82</v>
+      </c>
+      <c r="K170">
+        <v>4.0520930000000002</v>
+      </c>
+      <c r="P170">
+        <v>7</v>
+      </c>
+      <c r="Q170">
+        <v>3.4923329999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D171">
+        <v>8</v>
+      </c>
+      <c r="E171">
+        <v>3.4986649999999999</v>
+      </c>
+      <c r="F171">
+        <v>33</v>
+      </c>
+      <c r="G171">
+        <v>3.661524</v>
+      </c>
+      <c r="H171">
+        <v>58</v>
+      </c>
+      <c r="I171">
+        <v>3.8074910000000002</v>
+      </c>
+      <c r="J171">
+        <v>83</v>
+      </c>
+      <c r="K171">
+        <v>4.063879</v>
+      </c>
+      <c r="P171">
+        <v>8</v>
+      </c>
+      <c r="Q171">
+        <v>3.4986649999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D172">
+        <v>9</v>
+      </c>
+      <c r="E172">
+        <v>3.5051670000000001</v>
+      </c>
+      <c r="F172">
+        <v>34</v>
+      </c>
+      <c r="G172">
+        <v>3.6656279999999999</v>
+      </c>
+      <c r="H172">
+        <v>59</v>
+      </c>
+      <c r="I172">
+        <v>3.8157480000000001</v>
+      </c>
+      <c r="J172">
+        <v>84</v>
+      </c>
+      <c r="K172">
+        <v>4.075736</v>
+      </c>
+      <c r="P172">
+        <v>9</v>
+      </c>
+      <c r="Q172">
+        <v>3.5051670000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D173">
+        <v>10</v>
+      </c>
+      <c r="E173">
+        <v>3.5121000000000002</v>
+      </c>
+      <c r="F173">
+        <v>35</v>
+      </c>
+      <c r="G173">
+        <v>3.6697329999999999</v>
+      </c>
+      <c r="H173">
+        <v>60</v>
+      </c>
+      <c r="I173">
+        <v>3.8251330000000001</v>
+      </c>
+      <c r="J173">
+        <v>85</v>
+      </c>
+      <c r="K173">
+        <v>4.0872869999999999</v>
+      </c>
+      <c r="P173">
+        <v>10</v>
+      </c>
+      <c r="Q173">
+        <v>3.5121000000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D174">
+        <v>11</v>
+      </c>
+      <c r="E174">
+        <v>3.518983</v>
+      </c>
+      <c r="F174">
+        <v>36</v>
+      </c>
+      <c r="G174">
+        <v>3.6741440000000001</v>
+      </c>
+      <c r="H174">
+        <v>61</v>
+      </c>
+      <c r="I174">
+        <v>3.8339430000000001</v>
+      </c>
+      <c r="J174">
+        <v>86</v>
+      </c>
+      <c r="K174">
+        <v>4.0992829999999998</v>
+      </c>
+      <c r="P174">
+        <v>11</v>
+      </c>
+      <c r="Q174">
+        <v>3.518983</v>
+      </c>
+    </row>
+    <row r="175" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D175">
+        <v>12</v>
+      </c>
+      <c r="E175">
+        <v>3.5258820000000002</v>
+      </c>
+      <c r="F175">
+        <v>37</v>
+      </c>
+      <c r="G175">
+        <v>3.6783809999999999</v>
+      </c>
+      <c r="H175">
+        <v>62</v>
+      </c>
+      <c r="I175">
+        <v>3.8435790000000001</v>
+      </c>
+      <c r="J175">
+        <v>87</v>
+      </c>
+      <c r="K175">
+        <v>4.1116109999999999</v>
+      </c>
+      <c r="P175">
+        <v>12</v>
+      </c>
+      <c r="Q175">
+        <v>3.5258820000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D176">
+        <v>13</v>
+      </c>
+      <c r="E176">
+        <v>3.533115</v>
+      </c>
+      <c r="F176">
+        <v>38</v>
+      </c>
+      <c r="G176">
+        <v>3.6827390000000002</v>
+      </c>
+      <c r="H176">
+        <v>63</v>
+      </c>
+      <c r="I176">
+        <v>3.8529080000000002</v>
+      </c>
+      <c r="J176">
+        <v>88</v>
+      </c>
+      <c r="K176">
+        <v>4.1237729999999999</v>
+      </c>
+      <c r="P176">
+        <v>13</v>
+      </c>
+      <c r="Q176">
+        <v>3.533115</v>
+      </c>
+    </row>
+    <row r="177" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D177">
+        <v>14</v>
+      </c>
+      <c r="E177">
+        <v>3.541426</v>
+      </c>
+      <c r="F177">
+        <v>39</v>
+      </c>
+      <c r="G177">
+        <v>3.6873710000000002</v>
+      </c>
+      <c r="H177">
+        <v>64</v>
+      </c>
+      <c r="I177">
+        <v>3.8626680000000002</v>
+      </c>
+      <c r="J177">
+        <v>89</v>
+      </c>
+      <c r="K177">
+        <v>4.1360049999999999</v>
+      </c>
+      <c r="P177">
+        <v>14</v>
+      </c>
+      <c r="Q177">
+        <v>3.541426</v>
+      </c>
+    </row>
+    <row r="178" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D178">
+        <v>15</v>
+      </c>
+      <c r="E178">
+        <v>3.5503450000000001</v>
+      </c>
+      <c r="F178">
+        <v>40</v>
+      </c>
+      <c r="G178">
+        <v>3.6918000000000002</v>
+      </c>
+      <c r="H178">
+        <v>65</v>
+      </c>
+      <c r="I178">
+        <v>3.8725390000000002</v>
+      </c>
+      <c r="J178">
+        <v>90</v>
+      </c>
+      <c r="K178">
+        <v>4.1484990000000002</v>
+      </c>
+      <c r="P178">
+        <v>15</v>
+      </c>
+      <c r="Q178">
+        <v>3.5503450000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>16</v>
+      </c>
+      <c r="E179">
+        <v>3.5596830000000002</v>
+      </c>
+      <c r="F179">
+        <v>41</v>
+      </c>
+      <c r="G179">
+        <v>3.6964260000000002</v>
+      </c>
+      <c r="H179">
+        <v>66</v>
+      </c>
+      <c r="I179">
+        <v>3.8825910000000001</v>
+      </c>
+      <c r="J179">
+        <v>91</v>
+      </c>
+      <c r="K179">
+        <v>4.1610300000000002</v>
+      </c>
+      <c r="P179">
+        <v>16</v>
+      </c>
+      <c r="Q179">
+        <v>3.5596830000000002</v>
+      </c>
+    </row>
+    <row r="180" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D180">
+        <v>17</v>
+      </c>
+      <c r="E180">
+        <v>3.5688110000000002</v>
+      </c>
+      <c r="F180">
+        <v>42</v>
+      </c>
+      <c r="G180">
+        <v>3.7016909999999998</v>
+      </c>
+      <c r="H180">
+        <v>67</v>
+      </c>
+      <c r="I180">
+        <v>3.8923559999999999</v>
+      </c>
+      <c r="J180">
+        <v>92</v>
+      </c>
+      <c r="K180">
+        <v>4.1737729999999997</v>
+      </c>
+      <c r="P180">
+        <v>17</v>
+      </c>
+      <c r="Q180">
+        <v>3.5688110000000002</v>
+      </c>
+    </row>
+    <row r="181" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D181">
+        <v>18</v>
+      </c>
+      <c r="E181">
+        <v>3.5781299999999998</v>
+      </c>
+      <c r="F181">
+        <v>43</v>
+      </c>
+      <c r="G181">
+        <v>3.7068789999999998</v>
+      </c>
+      <c r="H181">
+        <v>68</v>
+      </c>
+      <c r="I181">
+        <v>3.9026320000000001</v>
+      </c>
+      <c r="J181">
+        <v>93</v>
+      </c>
+      <c r="K181">
+        <v>4.1867080000000003</v>
+      </c>
+      <c r="P181">
+        <v>18</v>
+      </c>
+      <c r="Q181">
+        <v>3.5781299999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D182">
+        <v>19</v>
+      </c>
+      <c r="E182">
+        <v>3.5870760000000002</v>
+      </c>
+      <c r="F182">
+        <v>44</v>
+      </c>
+      <c r="G182">
+        <v>3.7122130000000002</v>
+      </c>
+      <c r="H182">
+        <v>69</v>
+      </c>
+      <c r="I182">
+        <v>3.9126699999999999</v>
+      </c>
+      <c r="J182">
+        <v>94</v>
+      </c>
+      <c r="K182">
+        <v>4.1996310000000001</v>
+      </c>
+      <c r="P182">
+        <v>19</v>
+      </c>
+      <c r="Q182">
+        <v>3.5870760000000002</v>
+      </c>
+    </row>
+    <row r="183" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D183">
+        <v>20</v>
+      </c>
+      <c r="E183">
+        <v>3.5958990000000002</v>
+      </c>
+      <c r="F183">
+        <v>45</v>
+      </c>
+      <c r="G183">
+        <v>3.7175470000000002</v>
+      </c>
+      <c r="H183">
+        <v>70</v>
+      </c>
+      <c r="I183">
+        <v>3.9228160000000001</v>
+      </c>
+      <c r="J183">
+        <v>95</v>
+      </c>
+      <c r="K183">
+        <v>4.2</v>
+      </c>
+      <c r="P183">
+        <v>20</v>
+      </c>
+      <c r="Q183">
+        <v>3.5958990000000002</v>
+      </c>
+    </row>
+    <row r="184" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D184">
+        <v>21</v>
+      </c>
+      <c r="E184">
+        <v>3.6044960000000001</v>
+      </c>
+      <c r="F184">
+        <v>46</v>
+      </c>
+      <c r="G184">
+        <v>3.7231869999999998</v>
+      </c>
+      <c r="H184">
+        <v>71</v>
+      </c>
+      <c r="I184">
+        <v>3.9329779999999999</v>
+      </c>
+      <c r="J184">
+        <v>96</v>
+      </c>
+      <c r="K184">
+        <v>4.2</v>
+      </c>
+      <c r="P184">
+        <v>21</v>
+      </c>
+      <c r="Q184">
+        <v>3.6044960000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D185">
+        <v>22</v>
+      </c>
+      <c r="E185">
+        <v>3.6123430000000001</v>
+      </c>
+      <c r="F185">
+        <v>47</v>
+      </c>
+      <c r="G185">
+        <v>3.729136</v>
+      </c>
+      <c r="H185">
+        <v>72</v>
+      </c>
+      <c r="I185">
+        <v>3.9435959999999999</v>
+      </c>
+      <c r="J185">
+        <v>97</v>
+      </c>
+      <c r="K185">
+        <v>4.2</v>
+      </c>
+      <c r="P185">
+        <v>22</v>
+      </c>
+      <c r="Q185">
+        <v>3.6123430000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D186">
+        <v>23</v>
+      </c>
+      <c r="E186">
+        <v>3.618935</v>
+      </c>
+      <c r="F186">
+        <v>48</v>
+      </c>
+      <c r="G186">
+        <v>3.735087</v>
+      </c>
+      <c r="H186">
+        <v>73</v>
+      </c>
+      <c r="I186">
+        <v>3.9539240000000002</v>
+      </c>
+      <c r="J186">
+        <v>98</v>
+      </c>
+      <c r="K186">
+        <v>4.2</v>
+      </c>
+      <c r="P186">
+        <v>23</v>
+      </c>
+      <c r="Q186">
+        <v>3.618935</v>
+      </c>
+    </row>
+    <row r="187" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D187">
+        <v>24</v>
+      </c>
+      <c r="E187">
+        <v>3.6247229999999999</v>
+      </c>
+      <c r="F187">
+        <v>49</v>
+      </c>
+      <c r="G187">
+        <v>3.7408130000000002</v>
+      </c>
+      <c r="H187">
+        <v>74</v>
+      </c>
+      <c r="I187">
+        <v>3.9642330000000001</v>
+      </c>
+      <c r="J187">
+        <v>99</v>
+      </c>
+      <c r="K187">
+        <v>4.2</v>
+      </c>
+      <c r="P187">
+        <v>24</v>
+      </c>
+      <c r="Q187">
+        <v>3.6247229999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="J188">
+        <v>100</v>
+      </c>
+      <c r="K188">
+        <v>4.2</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="Q188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P189">
+        <v>25</v>
+      </c>
+      <c r="Q189">
+        <v>3.6292970000000002</v>
+      </c>
+    </row>
+    <row r="190" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P190">
+        <v>26</v>
+      </c>
+      <c r="Q190">
+        <v>3.6335190000000002</v>
+      </c>
+    </row>
+    <row r="191" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P191">
+        <v>27</v>
+      </c>
+      <c r="Q191">
+        <v>3.637324</v>
+      </c>
+    </row>
+    <row r="192" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P192">
+        <v>28</v>
+      </c>
+      <c r="Q192">
+        <v>3.6413039999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P193">
+        <v>29</v>
+      </c>
+      <c r="Q193">
+        <v>3.64567</v>
+      </c>
+    </row>
+    <row r="194" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P194">
+        <v>30</v>
+      </c>
+      <c r="Q194">
+        <v>3.6493099999999998</v>
+      </c>
+    </row>
+    <row r="195" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P195">
+        <v>31</v>
+      </c>
+      <c r="Q195">
+        <v>3.6531560000000001</v>
+      </c>
+    </row>
+    <row r="196" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P196">
+        <v>32</v>
+      </c>
+      <c r="Q196">
+        <v>3.6569940000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P197">
+        <v>33</v>
+      </c>
+      <c r="Q197">
+        <v>3.661524</v>
+      </c>
+    </row>
+    <row r="198" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P198">
+        <v>34</v>
+      </c>
+      <c r="Q198">
+        <v>3.6656279999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P199">
+        <v>35</v>
+      </c>
+      <c r="Q199">
+        <v>3.6697329999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P200">
+        <v>36</v>
+      </c>
+      <c r="Q200">
+        <v>3.6741440000000001</v>
+      </c>
+    </row>
+    <row r="201" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P201">
+        <v>37</v>
+      </c>
+      <c r="Q201">
+        <v>3.6783809999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P202">
+        <v>38</v>
+      </c>
+      <c r="Q202">
+        <v>3.6827390000000002</v>
+      </c>
+    </row>
+    <row r="203" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P203">
+        <v>39</v>
+      </c>
+      <c r="Q203">
+        <v>3.6873710000000002</v>
+      </c>
+    </row>
+    <row r="204" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P204">
+        <v>40</v>
+      </c>
+      <c r="Q204">
+        <v>3.6918000000000002</v>
+      </c>
+    </row>
+    <row r="205" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P205">
+        <v>41</v>
+      </c>
+      <c r="Q205">
+        <v>3.6964260000000002</v>
+      </c>
+    </row>
+    <row r="206" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P206">
+        <v>42</v>
+      </c>
+      <c r="Q206">
+        <v>3.7016909999999998</v>
+      </c>
+    </row>
+    <row r="207" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P207">
+        <v>43</v>
+      </c>
+      <c r="Q207">
+        <v>3.7068789999999998</v>
+      </c>
+    </row>
+    <row r="208" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P208">
+        <v>44</v>
+      </c>
+      <c r="Q208">
+        <v>3.7122130000000002</v>
+      </c>
+    </row>
+    <row r="209" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P209">
+        <v>45</v>
+      </c>
+      <c r="Q209">
+        <v>3.7175470000000002</v>
+      </c>
+    </row>
+    <row r="210" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P210">
+        <v>46</v>
+      </c>
+      <c r="Q210">
+        <v>3.7231869999999998</v>
+      </c>
+    </row>
+    <row r="211" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P211">
+        <v>47</v>
+      </c>
+      <c r="Q211">
+        <v>3.729136</v>
+      </c>
+    </row>
+    <row r="212" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P212">
+        <v>48</v>
+      </c>
+      <c r="Q212">
+        <v>3.735087</v>
+      </c>
+    </row>
+    <row r="213" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P213">
+        <v>49</v>
+      </c>
+      <c r="Q213">
+        <v>3.7408130000000002</v>
+      </c>
+    </row>
+    <row r="214" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P214">
+        <v>0</v>
+      </c>
+      <c r="Q214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P215">
+        <v>50</v>
+      </c>
+      <c r="Q215">
+        <v>3.7472940000000001</v>
+      </c>
+    </row>
+    <row r="216" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P216">
+        <v>51</v>
+      </c>
+      <c r="Q216">
+        <v>3.7538320000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P217">
+        <v>52</v>
+      </c>
+      <c r="Q217">
+        <v>3.7604199999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P218">
+        <v>53</v>
+      </c>
+      <c r="Q218">
+        <v>3.7674280000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P219">
+        <v>54</v>
+      </c>
+      <c r="Q219">
+        <v>3.774896</v>
+      </c>
+    </row>
+    <row r="220" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P220">
+        <v>55</v>
+      </c>
+      <c r="Q220">
+        <v>3.7825730000000002</v>
+      </c>
+    </row>
+    <row r="221" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P221">
+        <v>56</v>
+      </c>
+      <c r="Q221">
+        <v>3.7906659999999999</v>
+      </c>
+    </row>
+    <row r="222" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P222">
+        <v>57</v>
+      </c>
+      <c r="Q222">
+        <v>3.7990330000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P223">
+        <v>58</v>
+      </c>
+      <c r="Q223">
+        <v>3.8074910000000002</v>
+      </c>
+    </row>
+    <row r="224" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P224">
+        <v>59</v>
+      </c>
+      <c r="Q224">
+        <v>3.8157480000000001</v>
+      </c>
+    </row>
+    <row r="225" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P225">
+        <v>60</v>
+      </c>
+      <c r="Q225">
+        <v>3.8251330000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P226">
+        <v>61</v>
+      </c>
+      <c r="Q226">
+        <v>3.8339430000000001</v>
+      </c>
+    </row>
+    <row r="227" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P227">
+        <v>62</v>
+      </c>
+      <c r="Q227">
+        <v>3.8435790000000001</v>
+      </c>
+    </row>
+    <row r="228" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P228">
+        <v>63</v>
+      </c>
+      <c r="Q228">
+        <v>3.8529080000000002</v>
+      </c>
+    </row>
+    <row r="229" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P229">
+        <v>64</v>
+      </c>
+      <c r="Q229">
+        <v>3.8626680000000002</v>
+      </c>
+    </row>
+    <row r="230" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P230">
+        <v>65</v>
+      </c>
+      <c r="Q230">
+        <v>3.8725390000000002</v>
+      </c>
+    </row>
+    <row r="231" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P231">
+        <v>66</v>
+      </c>
+      <c r="Q231">
+        <v>3.8825910000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P232">
+        <v>67</v>
+      </c>
+      <c r="Q232">
+        <v>3.8923559999999999</v>
+      </c>
+    </row>
+    <row r="233" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P233">
+        <v>68</v>
+      </c>
+      <c r="Q233">
+        <v>3.9026320000000001</v>
+      </c>
+    </row>
+    <row r="234" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P234">
+        <v>69</v>
+      </c>
+      <c r="Q234">
+        <v>3.9126699999999999</v>
+      </c>
+    </row>
+    <row r="235" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P235">
+        <v>70</v>
+      </c>
+      <c r="Q235">
+        <v>3.9228160000000001</v>
+      </c>
+    </row>
+    <row r="236" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P236">
+        <v>71</v>
+      </c>
+      <c r="Q236">
+        <v>3.9329779999999999</v>
+      </c>
+    </row>
+    <row r="237" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P237">
+        <v>72</v>
+      </c>
+      <c r="Q237">
+        <v>3.9435959999999999</v>
+      </c>
+    </row>
+    <row r="238" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P238">
+        <v>73</v>
+      </c>
+      <c r="Q238">
+        <v>3.9539240000000002</v>
+      </c>
+    </row>
+    <row r="239" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P239">
+        <v>74</v>
+      </c>
+      <c r="Q239">
+        <v>3.9642330000000001</v>
+      </c>
+    </row>
+    <row r="240" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P240">
+        <v>0</v>
+      </c>
+      <c r="Q240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P241">
+        <v>75</v>
+      </c>
+      <c r="Q241">
+        <v>3.9751690000000002</v>
+      </c>
+    </row>
+    <row r="242" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P242">
+        <v>76</v>
+      </c>
+      <c r="Q242">
+        <v>3.9859170000000002</v>
+      </c>
+    </row>
+    <row r="243" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P243">
+        <v>77</v>
+      </c>
+      <c r="Q243">
+        <v>3.9967329999999999</v>
+      </c>
+    </row>
+    <row r="244" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P244">
+        <v>78</v>
+      </c>
+      <c r="Q244">
+        <v>4.0076650000000003</v>
+      </c>
+    </row>
+    <row r="245" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P245">
+        <v>79</v>
+      </c>
+      <c r="Q245">
+        <v>4.0185440000000003</v>
+      </c>
+    </row>
+    <row r="246" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P246">
+        <v>80</v>
+      </c>
+      <c r="Q246">
+        <v>4.0295370000000004</v>
+      </c>
+    </row>
+    <row r="247" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P247">
+        <v>81</v>
+      </c>
+      <c r="Q247">
+        <v>4.041086</v>
+      </c>
+    </row>
+    <row r="248" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P248">
+        <v>82</v>
+      </c>
+      <c r="Q248">
+        <v>4.0520930000000002</v>
+      </c>
+    </row>
+    <row r="249" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P249">
+        <v>83</v>
+      </c>
+      <c r="Q249">
+        <v>4.063879</v>
+      </c>
+    </row>
+    <row r="250" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P250">
+        <v>84</v>
+      </c>
+      <c r="Q250">
+        <v>4.075736</v>
+      </c>
+    </row>
+    <row r="251" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P251">
+        <v>85</v>
+      </c>
+      <c r="Q251">
+        <v>4.0872869999999999</v>
+      </c>
+    </row>
+    <row r="252" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P252">
+        <v>86</v>
+      </c>
+      <c r="Q252">
+        <v>4.0992829999999998</v>
+      </c>
+    </row>
+    <row r="253" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P253">
+        <v>87</v>
+      </c>
+      <c r="Q253">
+        <v>4.1116109999999999</v>
+      </c>
+    </row>
+    <row r="254" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P254">
+        <v>88</v>
+      </c>
+      <c r="Q254">
+        <v>4.1237729999999999</v>
+      </c>
+    </row>
+    <row r="255" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P255">
+        <v>89</v>
+      </c>
+      <c r="Q255">
+        <v>4.1360049999999999</v>
+      </c>
+    </row>
+    <row r="256" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P256">
+        <v>90</v>
+      </c>
+      <c r="Q256">
+        <v>4.1484990000000002</v>
+      </c>
+    </row>
+    <row r="257" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P257">
+        <v>91</v>
+      </c>
+      <c r="Q257">
+        <v>4.1610300000000002</v>
+      </c>
+    </row>
+    <row r="258" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P258">
+        <v>92</v>
+      </c>
+      <c r="Q258">
+        <v>4.1737729999999997</v>
+      </c>
+    </row>
+    <row r="259" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P259">
+        <v>93</v>
+      </c>
+      <c r="Q259">
+        <v>4.1867080000000003</v>
+      </c>
+    </row>
+    <row r="260" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P260">
+        <v>94</v>
+      </c>
+      <c r="Q260">
+        <v>4.1996310000000001</v>
+      </c>
+    </row>
+    <row r="261" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P261">
+        <v>95</v>
+      </c>
+      <c r="Q261">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="262" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P262">
+        <v>96</v>
+      </c>
+      <c r="Q262">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="263" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P263">
+        <v>97</v>
+      </c>
+      <c r="Q263">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="264" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P264">
+        <v>98</v>
+      </c>
+      <c r="Q264">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="265" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P265">
+        <v>99</v>
+      </c>
+      <c r="Q265">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="266" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P266">
+        <v>100</v>
+      </c>
+      <c r="Q266">
+        <v>4.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>

</xml_diff>

<commit_message>
Add Stack and Unstack Commands
Very interesting use of REDUCE function. Excellent drill.
</commit_message>
<xml_diff>
--- a/UnwrapAnArray.xlsx
+++ b/UnwrapAnArray.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{08AD3DBE-035A-406A-9BB9-F1005714D6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19BB00B7-B074-4470-BFA3-02D011E1E454}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="8_{08AD3DBE-035A-406A-9BB9-F1005714D6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F65ED6EF-B2A5-4437-B159-DDE19B500776}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="2" r:id="rId1"/>
     <sheet name="InterestingFormula" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Stacker" sheetId="3" r:id="rId3"/>
+    <sheet name="Unstacker" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Table1!$A$1:$F$6</definedName>
     <definedName name="SplitCols">_xlfn.LAMBDA(_xlpm.array,_xlpm.start,_xlpm.end,_xlfn.TAKE(_xlfn.DROP(_xlpm.array,,_xlpm.start-1),,_xlpm.end-_xlpm.start+1))</definedName>
+    <definedName name="SplitRows">_xlfn.LAMBDA(_xlpm.array,_xlpm.t,_xlpm.b,_xlfn.DROP(_xlfn.DROP(_xlpm.array,_xlpm.b-ROWS(_xlpm.array)),_xlpm.t-1))</definedName>
     <definedName name="Stacker">_xlfn.LAMBDA(_xlpm.array,_xlfn.DROP(_xlfn.REDUCE({0,0},_xlfn.SEQUENCE(,COLUMNS(_xlpm.array)/2,1,2),_xlfn.LAMBDA(_xlpm.x,_xlpm.y, _xlfn.VSTACK(_xlpm.x,SplitCols(_xlpm.array,_xlpm.y,_xlpm.y+1)))),1))</definedName>
     <definedName name="Stacker2">_xlfn.LAMBDA(_xlpm.array,_xlpm.cols,    _xlfn.DROP(      _xlfn.REDUCE(        _xlfn.SEQUENCE(,_xlpm.cols,0,0),        _xlfn.SEQUENCE(          ,          COLUMNS(            _xlpm.array)/_xlpm.cols,1,_xlpm.cols),        _xlfn.LAMBDA(_xlpm.x,_xlpm.y,          _xlfn.VSTACK(            _xlpm.x,            SplitCols(              _xlpm.array,_xlpm.y,_xlpm.y+_xlpm.cols-1)))),1))</definedName>
+    <definedName name="Unstack">_xlfn.LAMBDA(_xlpm.array,_xlpm.rws,        _xlfn.DROP(_xlfn.REDUCE(             _xlfn.SEQUENCE(_xlpm.rws,,0,0),             _xlfn.SEQUENCE(ROWS(_xlpm.array)/_xlpm.rws,,1,_xlpm.rws),             _xlfn.LAMBDA(_xlpm.x,_xlpm.y,                  _xlfn.HSTACK(_xlpm.x,                     SplitRows(                          _xlpm.array, _xlpm.y,_xlpm.y+_xlpm.rws-1                      ))              ) ),,1))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -89,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="60">
   <si>
     <t>FROM:</t>
   </si>
@@ -267,6 +270,9 @@
   <si>
     <t>Arbitrary Length Column Stacker</t>
   </si>
+  <si>
+    <t>Unstack an array</t>
+  </si>
 </sst>
 </file>
 
@@ -441,13 +447,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -591,9 +600,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>478478</xdr:colOff>
+      <xdr:colOff>474668</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>135634</xdr:rowOff>
+      <xdr:rowOff>131824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -618,6 +627,143 @@
         <a:xfrm>
           <a:off x="11582400" y="1552575"/>
           <a:ext cx="2314898" cy="2715004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>320426</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BE37CA8-DF13-E915-99F4-177C04E42446}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14630400" y="1552575"/>
+          <a:ext cx="2762636" cy="2991267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>398145</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>116591</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>116622</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E4B04E-8264-F6F5-41A9-672B8AB08754}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14418945" y="1592580"/>
+          <a:ext cx="2766446" cy="2991267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>495709</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9837</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DB4C83-03C1-2B5C-E40A-D652609BD3BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="514350"/>
+          <a:ext cx="2934109" cy="2238687"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -752,6 +898,18 @@
     <tableColumn id="10" xr3:uid="{A1B4D0C5-0C7B-4101-8A1A-5970BAE81642}" name="Col10"/>
     <tableColumn id="11" xr3:uid="{B60DC55E-800B-49B9-9262-E42DB981178B}" name="Col11"/>
     <tableColumn id="12" xr3:uid="{64AB61C1-44B6-4CF6-ADC8-3187DBE6D981}" name="Col12"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8A041A3D-AA73-4545-817C-F5644B6A18C0}" name="Table4" displayName="Table4" ref="B7:D19" totalsRowShown="0">
+  <autoFilter ref="B7:D19" xr:uid="{8A041A3D-AA73-4545-817C-F5644B6A18C0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D1F99C6F-379D-4C02-B6EF-F33C50338204}" name="Col1"/>
+    <tableColumn id="2" xr3:uid="{6E21181D-D8A4-4783-B71F-C0BAC58C39AC}" name="Col2"/>
+    <tableColumn id="3" xr3:uid="{876111BF-CC04-4D5A-932A-CC916BA61513}" name="Col3"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1931,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296D7A3E-D33F-49E4-A212-60F607EA8E1E}">
   <dimension ref="A1:AB266"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61:Q160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2341,7 +2499,7 @@
         <v>B</v>
       </c>
       <c r="Q34" t="str" cm="1">
-        <f t="array" ref="Q34:R51">_xlfn.LAMBDA(_xlpm.array,_xlpm.cols,
+        <f t="array" ref="Q34:S45">_xlfn.LAMBDA(_xlpm.array,_xlpm.cols,
    _xlfn.DROP(
      _xlfn.REDUCE(
        _xlfn.SEQUENCE(,_xlpm.cols,0,0),
@@ -2353,11 +2511,14 @@
          _xlfn.VSTACK(
            _xlpm.x,
            SplitCols(
-             _xlpm.array,_xlpm.y,_xlpm.y+_xlpm.cols-1)))),1))(_tTest[],2)</f>
+             _xlpm.array,_xlpm.y,_xlpm.y+_xlpm.cols-1)))),1))(_tTest[],3)</f>
         <v>A</v>
       </c>
       <c r="R34" t="str">
         <v>B</v>
+      </c>
+      <c r="S34" t="str">
+        <v>C</v>
       </c>
       <c r="X34" t="str" cm="1">
         <f t="array" ref="X34:AB39">Stacker2(_tTest[],5)</f>
@@ -2395,6 +2556,9 @@
       <c r="R35" t="str">
         <v>H</v>
       </c>
+      <c r="S35" t="str">
+        <v>I</v>
+      </c>
       <c r="X35" t="str">
         <v>G</v>
       </c>
@@ -2430,6 +2594,9 @@
       <c r="R36" t="str">
         <v>N</v>
       </c>
+      <c r="S36" t="str">
+        <v>O</v>
+      </c>
       <c r="X36" t="str">
         <v>M</v>
       </c>
@@ -2460,10 +2627,13 @@
         <v>D</v>
       </c>
       <c r="Q37" t="str">
-        <v>C</v>
+        <v>D</v>
       </c>
       <c r="R37" t="str">
-        <v>D</v>
+        <v>E</v>
+      </c>
+      <c r="S37" t="str">
+        <v>F</v>
       </c>
       <c r="X37" t="str">
         <v>F</v>
@@ -2495,10 +2665,13 @@
         <v>J</v>
       </c>
       <c r="Q38" t="str">
-        <v>I</v>
+        <v>J</v>
       </c>
       <c r="R38" t="str">
-        <v>J</v>
+        <v>K</v>
+      </c>
+      <c r="S38" t="str">
+        <v>L</v>
       </c>
       <c r="X38" t="str">
         <v>L</v>
@@ -2530,10 +2703,13 @@
         <v>P</v>
       </c>
       <c r="Q39" t="str">
-        <v>O</v>
+        <v>P</v>
       </c>
       <c r="R39" t="str">
-        <v>P</v>
+        <v>Q</v>
+      </c>
+      <c r="S39" t="str">
+        <v>R</v>
       </c>
       <c r="X39" t="str">
         <v>R</v>
@@ -2564,11 +2740,14 @@
       <c r="M40" t="str">
         <v>F</v>
       </c>
-      <c r="Q40" t="str">
-        <v>E</v>
-      </c>
-      <c r="R40" t="str">
-        <v>F</v>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>4</v>
+      </c>
+      <c r="S40" t="str">
+        <v>aa</v>
       </c>
     </row>
     <row r="41" spans="9:28" x14ac:dyDescent="0.25">
@@ -2584,11 +2763,14 @@
       <c r="M41" t="str">
         <v>L</v>
       </c>
-      <c r="Q41" t="str">
-        <v>K</v>
-      </c>
-      <c r="R41" t="str">
-        <v>L</v>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41">
+        <v>5</v>
+      </c>
+      <c r="S41" t="str">
+        <v>ab</v>
       </c>
     </row>
     <row r="42" spans="9:28" x14ac:dyDescent="0.25">
@@ -2604,11 +2786,14 @@
       <c r="M42" t="str">
         <v>R</v>
       </c>
-      <c r="Q42" t="str">
-        <v>Q</v>
-      </c>
-      <c r="R42" t="str">
-        <v>R</v>
+      <c r="Q42">
+        <v>3</v>
+      </c>
+      <c r="R42">
+        <v>6</v>
+      </c>
+      <c r="S42" t="str">
+        <v>ac</v>
       </c>
     </row>
     <row r="43" spans="9:28" x14ac:dyDescent="0.25">
@@ -2624,11 +2809,14 @@
       <c r="M43">
         <v>4</v>
       </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-      <c r="R43">
-        <v>4</v>
+      <c r="Q43" t="str">
+        <v>ad</v>
+      </c>
+      <c r="R43" t="str">
+        <v>zz</v>
+      </c>
+      <c r="S43" t="str">
+        <v>yy</v>
       </c>
     </row>
     <row r="44" spans="9:28" x14ac:dyDescent="0.25">
@@ -2644,11 +2832,14 @@
       <c r="M44">
         <v>5</v>
       </c>
-      <c r="Q44">
-        <v>2</v>
-      </c>
-      <c r="R44">
-        <v>5</v>
+      <c r="Q44" t="str">
+        <v>ae</v>
+      </c>
+      <c r="R44" t="str">
+        <v>zz</v>
+      </c>
+      <c r="S44" t="str">
+        <v>yy</v>
       </c>
     </row>
     <row r="45" spans="9:28" x14ac:dyDescent="0.25">
@@ -2664,11 +2855,14 @@
       <c r="M45">
         <v>6</v>
       </c>
-      <c r="Q45">
-        <v>3</v>
-      </c>
-      <c r="R45">
-        <v>6</v>
+      <c r="Q45" t="str">
+        <v>af</v>
+      </c>
+      <c r="R45" t="str">
+        <v>zz</v>
+      </c>
+      <c r="S45" t="str">
+        <v>yy</v>
       </c>
     </row>
     <row r="46" spans="9:28" x14ac:dyDescent="0.25">
@@ -2684,12 +2878,6 @@
       <c r="M46" t="str">
         <v>ad</v>
       </c>
-      <c r="Q46" t="str">
-        <v>aa</v>
-      </c>
-      <c r="R46" t="str">
-        <v>ad</v>
-      </c>
     </row>
     <row r="47" spans="9:28" x14ac:dyDescent="0.25">
       <c r="I47" t="str">
@@ -2704,12 +2892,6 @@
       <c r="M47" t="str">
         <v>ae</v>
       </c>
-      <c r="Q47" t="str">
-        <v>ab</v>
-      </c>
-      <c r="R47" t="str">
-        <v>ae</v>
-      </c>
     </row>
     <row r="48" spans="9:28" x14ac:dyDescent="0.25">
       <c r="I48" t="str">
@@ -2724,14 +2906,8 @@
       <c r="M48" t="str">
         <v>af</v>
       </c>
-      <c r="Q48" t="str">
-        <v>ac</v>
-      </c>
-      <c r="R48" t="str">
-        <v>af</v>
-      </c>
-    </row>
-    <row r="49" spans="5:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I49" t="str">
         <v>zz</v>
       </c>
@@ -2744,14 +2920,8 @@
       <c r="M49" t="str">
         <v>yy</v>
       </c>
-      <c r="Q49" t="str">
-        <v>zz</v>
-      </c>
-      <c r="R49" t="str">
-        <v>yy</v>
-      </c>
-    </row>
-    <row r="50" spans="5:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I50" t="str">
         <v>zz</v>
       </c>
@@ -2764,14 +2934,8 @@
       <c r="M50" t="str">
         <v>yy</v>
       </c>
-      <c r="Q50" t="str">
-        <v>zz</v>
-      </c>
-      <c r="R50" t="str">
-        <v>yy</v>
-      </c>
-    </row>
-    <row r="51" spans="5:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I51" t="str">
         <v>zz</v>
       </c>
@@ -2784,14 +2948,8 @@
       <c r="M51" t="str">
         <v>yy</v>
       </c>
-      <c r="Q51" t="str">
-        <v>zz</v>
-      </c>
-      <c r="R51" t="str">
-        <v>yy</v>
-      </c>
-    </row>
-    <row r="61" spans="5:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E61">
         <v>0</v>
       </c>
@@ -2824,7 +2982,7 @@
         <v>3.0822630000000002</v>
       </c>
     </row>
-    <row r="62" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E62">
         <v>1</v>
       </c>
@@ -2856,7 +3014,7 @@
         <v>3.2301890000000002</v>
       </c>
     </row>
-    <row r="63" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E63">
         <v>2</v>
       </c>
@@ -2888,7 +3046,7 @@
         <v>3.3168229999999999</v>
       </c>
     </row>
-    <row r="64" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E64">
         <v>3</v>
       </c>
@@ -5644,6 +5802,2100 @@
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7816223-0D42-4F27-8912-D53BDCF2DEF5}">
+  <dimension ref="A1:Y142"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>TEXT(DATE(2023,7,20),"dd-mmm-yyyy")</f>
+        <v>20-Jul-2023</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="str" cm="1">
+        <f t="array" ref="H7:J10">_xlfn.LAMBDA(_xlpm.array,_xlpm.t,_xlpm.b,_xlfn.DROP(_xlfn.DROP(Table4[],_xlpm.b-ROWS(_xlpm.array)),_xlpm.t-1))(Table4[],1,4)</f>
+        <v>A</v>
+      </c>
+      <c r="I7" t="str">
+        <v>B</v>
+      </c>
+      <c r="J7" t="str">
+        <v>C</v>
+      </c>
+      <c r="L7" t="str" cm="1">
+        <f t="array" ref="L7:N10">SplitRows(Table4[],2,5)</f>
+        <v>G</v>
+      </c>
+      <c r="M7" t="str">
+        <v>H</v>
+      </c>
+      <c r="N7" t="str">
+        <v>I</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="str">
+        <v>G</v>
+      </c>
+      <c r="I8" t="str">
+        <v>H</v>
+      </c>
+      <c r="J8" t="str">
+        <v>I</v>
+      </c>
+      <c r="L8" t="str">
+        <v>M</v>
+      </c>
+      <c r="M8" t="str">
+        <v>N</v>
+      </c>
+      <c r="N8" t="str">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="str">
+        <v>M</v>
+      </c>
+      <c r="I9" t="str">
+        <v>N</v>
+      </c>
+      <c r="J9" t="str">
+        <v>O</v>
+      </c>
+      <c r="L9" t="str">
+        <v>D</v>
+      </c>
+      <c r="M9" t="str">
+        <v>E</v>
+      </c>
+      <c r="N9" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="str">
+        <v>D</v>
+      </c>
+      <c r="I10" t="str">
+        <v>E</v>
+      </c>
+      <c r="J10" t="str">
+        <v>F</v>
+      </c>
+      <c r="L10" t="str">
+        <v>J</v>
+      </c>
+      <c r="M10" t="str">
+        <v>K</v>
+      </c>
+      <c r="N10" t="str">
+        <v>L</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" cm="1">
+        <f t="array" ref="H14:N19">_xlfn.LAMBDA(_xlpm.array,_xlpm.rws,
+       _xlfn.REDUCE(
+            _xlfn.SEQUENCE(_xlpm.rws,,0,0),
+            _xlfn.SEQUENCE(ROWS(_xlpm.array)/_xlpm.rws,,_xlpm.rws),
+            _xlfn.LAMBDA(_xlpm.x,_xlpm.y,
+                 _xlfn.HSTACK(
+                    SplitRows(
+                         _xlpm.array, _xlpm.y,_xlpm.y+_xlpm.rws-1
+                     ),_xlpm.x)
+             )
+))(Table4[],6)</f>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" t="str">
+        <v>aa</v>
+      </c>
+      <c r="K14" t="str">
+        <v>P</v>
+      </c>
+      <c r="L14" t="str">
+        <v>Q</v>
+      </c>
+      <c r="M14" t="str">
+        <v>R</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15" t="str">
+        <v>ab</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15" t="str">
+        <v>aa</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" t="str">
+        <v>ac</v>
+      </c>
+      <c r="K16" s="6">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16" t="str">
+        <v>ab</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" t="str">
+        <v>ad</v>
+      </c>
+      <c r="I17" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J17" t="str">
+        <v>yy</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>6</v>
+      </c>
+      <c r="M17" t="str">
+        <v>ac</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" t="str">
+        <v>ae</v>
+      </c>
+      <c r="I18" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J18" t="str">
+        <v>yy</v>
+      </c>
+      <c r="K18" t="str">
+        <v>ad</v>
+      </c>
+      <c r="L18" t="str">
+        <v>zz</v>
+      </c>
+      <c r="M18" t="str">
+        <v>yy</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" t="str">
+        <v>af</v>
+      </c>
+      <c r="I19" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J19" t="str">
+        <v>yy</v>
+      </c>
+      <c r="K19" t="str">
+        <v>ae</v>
+      </c>
+      <c r="L19" t="str">
+        <v>zz</v>
+      </c>
+      <c r="M19" t="str">
+        <v>yy</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H22" t="str" cm="1">
+        <f t="array" ref="H22:Y23">_xlfn.LAMBDA(_xlpm.array,_xlpm.rws,
+       _xlfn.DROP(_xlfn.REDUCE(
+            _xlfn.SEQUENCE(_xlpm.rws,,0,0),
+            _xlfn.SEQUENCE(ROWS(_xlpm.array)/_xlpm.rws,,1,_xlpm.rws),
+            _xlfn.LAMBDA(_xlpm.x,_xlpm.y,
+                 _xlfn.HSTACK(_xlpm.x,
+                    SplitRows(
+                         _xlpm.array, _xlpm.y,_xlpm.y+_xlpm.rws-1
+                     ))
+             )
+),,1))(Table4[],2)</f>
+        <v>A</v>
+      </c>
+      <c r="I22" t="str">
+        <v>B</v>
+      </c>
+      <c r="J22" t="str">
+        <v>C</v>
+      </c>
+      <c r="K22" t="str">
+        <v>M</v>
+      </c>
+      <c r="L22" t="str">
+        <v>N</v>
+      </c>
+      <c r="M22" t="str">
+        <v>O</v>
+      </c>
+      <c r="N22" t="str">
+        <v>J</v>
+      </c>
+      <c r="O22" t="str">
+        <v>K</v>
+      </c>
+      <c r="P22" t="str">
+        <v>L</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22" t="str">
+        <v>aa</v>
+      </c>
+      <c r="T22">
+        <v>3</v>
+      </c>
+      <c r="U22">
+        <v>6</v>
+      </c>
+      <c r="V22" t="str">
+        <v>ac</v>
+      </c>
+      <c r="W22" t="str">
+        <v>ae</v>
+      </c>
+      <c r="X22" t="str">
+        <v>zz</v>
+      </c>
+      <c r="Y22" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <v>G</v>
+      </c>
+      <c r="I23" t="str">
+        <v>H</v>
+      </c>
+      <c r="J23" t="str">
+        <v>I</v>
+      </c>
+      <c r="K23" t="str">
+        <v>D</v>
+      </c>
+      <c r="L23" t="str">
+        <v>E</v>
+      </c>
+      <c r="M23" t="str">
+        <v>F</v>
+      </c>
+      <c r="N23" t="str">
+        <v>P</v>
+      </c>
+      <c r="O23" t="str">
+        <v>Q</v>
+      </c>
+      <c r="P23" t="str">
+        <v>R</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
+      </c>
+      <c r="S23" t="str">
+        <v>ab</v>
+      </c>
+      <c r="T23" t="str">
+        <v>ad</v>
+      </c>
+      <c r="U23" t="str">
+        <v>zz</v>
+      </c>
+      <c r="V23" t="str">
+        <v>yy</v>
+      </c>
+      <c r="W23" t="str">
+        <v>af</v>
+      </c>
+      <c r="X23" t="str">
+        <v>zz</v>
+      </c>
+      <c r="Y23" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H26" t="str" cm="1">
+        <f t="array" ref="H26:J37">Unstack(Table4[],12)</f>
+        <v>A</v>
+      </c>
+      <c r="I26" t="str">
+        <v>B</v>
+      </c>
+      <c r="J26" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <v>G</v>
+      </c>
+      <c r="I27" t="str">
+        <v>H</v>
+      </c>
+      <c r="J27" t="str">
+        <v>I</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <v>M</v>
+      </c>
+      <c r="I28" t="str">
+        <v>N</v>
+      </c>
+      <c r="J28" t="str">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <v>D</v>
+      </c>
+      <c r="I29" t="str">
+        <v>E</v>
+      </c>
+      <c r="J29" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <v>J</v>
+      </c>
+      <c r="I30" t="str">
+        <v>K</v>
+      </c>
+      <c r="J30" t="str">
+        <v>L</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <v>P</v>
+      </c>
+      <c r="I31" t="str">
+        <v>Q</v>
+      </c>
+      <c r="J31" t="str">
+        <v>R</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32" t="str">
+        <v>aa</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33" t="str">
+        <v>ab</v>
+      </c>
+    </row>
+    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>3</v>
+      </c>
+      <c r="I34">
+        <v>6</v>
+      </c>
+      <c r="J34" t="str">
+        <v>ac</v>
+      </c>
+    </row>
+    <row r="35" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <v>ad</v>
+      </c>
+      <c r="I35" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J35" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="36" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <v>ae</v>
+      </c>
+      <c r="I36" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J36" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H37" t="str">
+        <v>af</v>
+      </c>
+      <c r="I37" t="str">
+        <v>zz</v>
+      </c>
+      <c r="J37" t="str">
+        <v>yy</v>
+      </c>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>3.0822630000000002</v>
+      </c>
+      <c r="H43" cm="1">
+        <f t="array" ref="H43:O67">Unstack(D43:E142,25)</f>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>3.0822630000000002</v>
+      </c>
+      <c r="J43">
+        <v>25</v>
+      </c>
+      <c r="K43">
+        <v>3.6292970000000002</v>
+      </c>
+      <c r="L43">
+        <v>50</v>
+      </c>
+      <c r="M43">
+        <v>3.7472940000000001</v>
+      </c>
+      <c r="N43">
+        <v>75</v>
+      </c>
+      <c r="O43">
+        <v>3.9751690000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>3.2301890000000002</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>3.2301890000000002</v>
+      </c>
+      <c r="J44">
+        <v>26</v>
+      </c>
+      <c r="K44">
+        <v>3.6335190000000002</v>
+      </c>
+      <c r="L44">
+        <v>51</v>
+      </c>
+      <c r="M44">
+        <v>3.7538320000000001</v>
+      </c>
+      <c r="N44">
+        <v>76</v>
+      </c>
+      <c r="O44">
+        <v>3.9859170000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>3.3168229999999999</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>3.3168229999999999</v>
+      </c>
+      <c r="J45">
+        <v>27</v>
+      </c>
+      <c r="K45">
+        <v>3.637324</v>
+      </c>
+      <c r="L45">
+        <v>52</v>
+      </c>
+      <c r="M45">
+        <v>3.7604199999999999</v>
+      </c>
+      <c r="N45">
+        <v>77</v>
+      </c>
+      <c r="O45">
+        <v>3.9967329999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>3.3811659999999999</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>3.3811659999999999</v>
+      </c>
+      <c r="J46">
+        <v>28</v>
+      </c>
+      <c r="K46">
+        <v>3.6413039999999999</v>
+      </c>
+      <c r="L46">
+        <v>53</v>
+      </c>
+      <c r="M46">
+        <v>3.7674280000000002</v>
+      </c>
+      <c r="N46">
+        <v>78</v>
+      </c>
+      <c r="O46">
+        <v>4.0076650000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>3.4311829999999999</v>
+      </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>3.4311829999999999</v>
+      </c>
+      <c r="J47">
+        <v>29</v>
+      </c>
+      <c r="K47">
+        <v>3.64567</v>
+      </c>
+      <c r="L47">
+        <v>54</v>
+      </c>
+      <c r="M47">
+        <v>3.774896</v>
+      </c>
+      <c r="N47">
+        <v>79</v>
+      </c>
+      <c r="O47">
+        <v>4.0185440000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>3.4698280000000001</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>3.4698280000000001</v>
+      </c>
+      <c r="J48">
+        <v>30</v>
+      </c>
+      <c r="K48">
+        <v>3.6493099999999998</v>
+      </c>
+      <c r="L48">
+        <v>55</v>
+      </c>
+      <c r="M48">
+        <v>3.7825730000000002</v>
+      </c>
+      <c r="N48">
+        <v>80</v>
+      </c>
+      <c r="O48">
+        <v>4.0295370000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49">
+        <v>3.4855589999999999</v>
+      </c>
+      <c r="H49">
+        <v>6</v>
+      </c>
+      <c r="I49">
+        <v>3.4855589999999999</v>
+      </c>
+      <c r="J49">
+        <v>31</v>
+      </c>
+      <c r="K49">
+        <v>3.6531560000000001</v>
+      </c>
+      <c r="L49">
+        <v>56</v>
+      </c>
+      <c r="M49">
+        <v>3.7906659999999999</v>
+      </c>
+      <c r="N49">
+        <v>81</v>
+      </c>
+      <c r="O49">
+        <v>4.041086</v>
+      </c>
+    </row>
+    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>3.4923329999999999</v>
+      </c>
+      <c r="H50">
+        <v>7</v>
+      </c>
+      <c r="I50">
+        <v>3.4923329999999999</v>
+      </c>
+      <c r="J50">
+        <v>32</v>
+      </c>
+      <c r="K50">
+        <v>3.6569940000000001</v>
+      </c>
+      <c r="L50">
+        <v>57</v>
+      </c>
+      <c r="M50">
+        <v>3.7990330000000001</v>
+      </c>
+      <c r="N50">
+        <v>82</v>
+      </c>
+      <c r="O50">
+        <v>4.0520930000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>8</v>
+      </c>
+      <c r="E51">
+        <v>3.4986649999999999</v>
+      </c>
+      <c r="H51">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <v>3.4986649999999999</v>
+      </c>
+      <c r="J51">
+        <v>33</v>
+      </c>
+      <c r="K51">
+        <v>3.661524</v>
+      </c>
+      <c r="L51">
+        <v>58</v>
+      </c>
+      <c r="M51">
+        <v>3.8074910000000002</v>
+      </c>
+      <c r="N51">
+        <v>83</v>
+      </c>
+      <c r="O51">
+        <v>4.063879</v>
+      </c>
+    </row>
+    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>9</v>
+      </c>
+      <c r="E52">
+        <v>3.5051670000000001</v>
+      </c>
+      <c r="H52">
+        <v>9</v>
+      </c>
+      <c r="I52">
+        <v>3.5051670000000001</v>
+      </c>
+      <c r="J52">
+        <v>34</v>
+      </c>
+      <c r="K52">
+        <v>3.6656279999999999</v>
+      </c>
+      <c r="L52">
+        <v>59</v>
+      </c>
+      <c r="M52">
+        <v>3.8157480000000001</v>
+      </c>
+      <c r="N52">
+        <v>84</v>
+      </c>
+      <c r="O52">
+        <v>4.075736</v>
+      </c>
+    </row>
+    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>3.5121000000000002</v>
+      </c>
+      <c r="H53">
+        <v>10</v>
+      </c>
+      <c r="I53">
+        <v>3.5121000000000002</v>
+      </c>
+      <c r="J53">
+        <v>35</v>
+      </c>
+      <c r="K53">
+        <v>3.6697329999999999</v>
+      </c>
+      <c r="L53">
+        <v>60</v>
+      </c>
+      <c r="M53">
+        <v>3.8251330000000001</v>
+      </c>
+      <c r="N53">
+        <v>85</v>
+      </c>
+      <c r="O53">
+        <v>4.0872869999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>11</v>
+      </c>
+      <c r="E54">
+        <v>3.518983</v>
+      </c>
+      <c r="H54">
+        <v>11</v>
+      </c>
+      <c r="I54">
+        <v>3.518983</v>
+      </c>
+      <c r="J54">
+        <v>36</v>
+      </c>
+      <c r="K54">
+        <v>3.6741440000000001</v>
+      </c>
+      <c r="L54">
+        <v>61</v>
+      </c>
+      <c r="M54">
+        <v>3.8339430000000001</v>
+      </c>
+      <c r="N54">
+        <v>86</v>
+      </c>
+      <c r="O54">
+        <v>4.0992829999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>12</v>
+      </c>
+      <c r="E55">
+        <v>3.5258820000000002</v>
+      </c>
+      <c r="H55">
+        <v>12</v>
+      </c>
+      <c r="I55">
+        <v>3.5258820000000002</v>
+      </c>
+      <c r="J55">
+        <v>37</v>
+      </c>
+      <c r="K55">
+        <v>3.6783809999999999</v>
+      </c>
+      <c r="L55">
+        <v>62</v>
+      </c>
+      <c r="M55">
+        <v>3.8435790000000001</v>
+      </c>
+      <c r="N55">
+        <v>87</v>
+      </c>
+      <c r="O55">
+        <v>4.1116109999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>13</v>
+      </c>
+      <c r="E56">
+        <v>3.533115</v>
+      </c>
+      <c r="H56">
+        <v>13</v>
+      </c>
+      <c r="I56">
+        <v>3.533115</v>
+      </c>
+      <c r="J56">
+        <v>38</v>
+      </c>
+      <c r="K56">
+        <v>3.6827390000000002</v>
+      </c>
+      <c r="L56">
+        <v>63</v>
+      </c>
+      <c r="M56">
+        <v>3.8529080000000002</v>
+      </c>
+      <c r="N56">
+        <v>88</v>
+      </c>
+      <c r="O56">
+        <v>4.1237729999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>14</v>
+      </c>
+      <c r="E57">
+        <v>3.541426</v>
+      </c>
+      <c r="H57">
+        <v>14</v>
+      </c>
+      <c r="I57">
+        <v>3.541426</v>
+      </c>
+      <c r="J57">
+        <v>39</v>
+      </c>
+      <c r="K57">
+        <v>3.6873710000000002</v>
+      </c>
+      <c r="L57">
+        <v>64</v>
+      </c>
+      <c r="M57">
+        <v>3.8626680000000002</v>
+      </c>
+      <c r="N57">
+        <v>89</v>
+      </c>
+      <c r="O57">
+        <v>4.1360049999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <v>3.5503450000000001</v>
+      </c>
+      <c r="H58">
+        <v>15</v>
+      </c>
+      <c r="I58">
+        <v>3.5503450000000001</v>
+      </c>
+      <c r="J58">
+        <v>40</v>
+      </c>
+      <c r="K58">
+        <v>3.6918000000000002</v>
+      </c>
+      <c r="L58">
+        <v>65</v>
+      </c>
+      <c r="M58">
+        <v>3.8725390000000002</v>
+      </c>
+      <c r="N58">
+        <v>90</v>
+      </c>
+      <c r="O58">
+        <v>4.1484990000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>16</v>
+      </c>
+      <c r="E59">
+        <v>3.5596830000000002</v>
+      </c>
+      <c r="H59">
+        <v>16</v>
+      </c>
+      <c r="I59">
+        <v>3.5596830000000002</v>
+      </c>
+      <c r="J59">
+        <v>41</v>
+      </c>
+      <c r="K59">
+        <v>3.6964260000000002</v>
+      </c>
+      <c r="L59">
+        <v>66</v>
+      </c>
+      <c r="M59">
+        <v>3.8825910000000001</v>
+      </c>
+      <c r="N59">
+        <v>91</v>
+      </c>
+      <c r="O59">
+        <v>4.1610300000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>17</v>
+      </c>
+      <c r="E60">
+        <v>3.5688110000000002</v>
+      </c>
+      <c r="H60">
+        <v>17</v>
+      </c>
+      <c r="I60">
+        <v>3.5688110000000002</v>
+      </c>
+      <c r="J60">
+        <v>42</v>
+      </c>
+      <c r="K60">
+        <v>3.7016909999999998</v>
+      </c>
+      <c r="L60">
+        <v>67</v>
+      </c>
+      <c r="M60">
+        <v>3.8923559999999999</v>
+      </c>
+      <c r="N60">
+        <v>92</v>
+      </c>
+      <c r="O60">
+        <v>4.1737729999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>18</v>
+      </c>
+      <c r="E61">
+        <v>3.5781299999999998</v>
+      </c>
+      <c r="H61">
+        <v>18</v>
+      </c>
+      <c r="I61">
+        <v>3.5781299999999998</v>
+      </c>
+      <c r="J61">
+        <v>43</v>
+      </c>
+      <c r="K61">
+        <v>3.7068789999999998</v>
+      </c>
+      <c r="L61">
+        <v>68</v>
+      </c>
+      <c r="M61">
+        <v>3.9026320000000001</v>
+      </c>
+      <c r="N61">
+        <v>93</v>
+      </c>
+      <c r="O61">
+        <v>4.1867080000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>19</v>
+      </c>
+      <c r="E62">
+        <v>3.5870760000000002</v>
+      </c>
+      <c r="H62">
+        <v>19</v>
+      </c>
+      <c r="I62">
+        <v>3.5870760000000002</v>
+      </c>
+      <c r="J62">
+        <v>44</v>
+      </c>
+      <c r="K62">
+        <v>3.7122130000000002</v>
+      </c>
+      <c r="L62">
+        <v>69</v>
+      </c>
+      <c r="M62">
+        <v>3.9126699999999999</v>
+      </c>
+      <c r="N62">
+        <v>94</v>
+      </c>
+      <c r="O62">
+        <v>4.1996310000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>20</v>
+      </c>
+      <c r="E63">
+        <v>3.5958990000000002</v>
+      </c>
+      <c r="H63">
+        <v>20</v>
+      </c>
+      <c r="I63">
+        <v>3.5958990000000002</v>
+      </c>
+      <c r="J63">
+        <v>45</v>
+      </c>
+      <c r="K63">
+        <v>3.7175470000000002</v>
+      </c>
+      <c r="L63">
+        <v>70</v>
+      </c>
+      <c r="M63">
+        <v>3.9228160000000001</v>
+      </c>
+      <c r="N63">
+        <v>95</v>
+      </c>
+      <c r="O63">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="64" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>21</v>
+      </c>
+      <c r="E64">
+        <v>3.6044960000000001</v>
+      </c>
+      <c r="H64">
+        <v>21</v>
+      </c>
+      <c r="I64">
+        <v>3.6044960000000001</v>
+      </c>
+      <c r="J64">
+        <v>46</v>
+      </c>
+      <c r="K64">
+        <v>3.7231869999999998</v>
+      </c>
+      <c r="L64">
+        <v>71</v>
+      </c>
+      <c r="M64">
+        <v>3.9329779999999999</v>
+      </c>
+      <c r="N64">
+        <v>96</v>
+      </c>
+      <c r="O64">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="65" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>22</v>
+      </c>
+      <c r="E65">
+        <v>3.6123430000000001</v>
+      </c>
+      <c r="H65">
+        <v>22</v>
+      </c>
+      <c r="I65">
+        <v>3.6123430000000001</v>
+      </c>
+      <c r="J65">
+        <v>47</v>
+      </c>
+      <c r="K65">
+        <v>3.729136</v>
+      </c>
+      <c r="L65">
+        <v>72</v>
+      </c>
+      <c r="M65">
+        <v>3.9435959999999999</v>
+      </c>
+      <c r="N65">
+        <v>97</v>
+      </c>
+      <c r="O65">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="66" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>23</v>
+      </c>
+      <c r="E66">
+        <v>3.618935</v>
+      </c>
+      <c r="H66">
+        <v>23</v>
+      </c>
+      <c r="I66">
+        <v>3.618935</v>
+      </c>
+      <c r="J66">
+        <v>48</v>
+      </c>
+      <c r="K66">
+        <v>3.735087</v>
+      </c>
+      <c r="L66">
+        <v>73</v>
+      </c>
+      <c r="M66">
+        <v>3.9539240000000002</v>
+      </c>
+      <c r="N66">
+        <v>98</v>
+      </c>
+      <c r="O66">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="67" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>24</v>
+      </c>
+      <c r="E67">
+        <v>3.6247229999999999</v>
+      </c>
+      <c r="H67">
+        <v>24</v>
+      </c>
+      <c r="I67">
+        <v>3.6247229999999999</v>
+      </c>
+      <c r="J67">
+        <v>49</v>
+      </c>
+      <c r="K67">
+        <v>3.7408130000000002</v>
+      </c>
+      <c r="L67">
+        <v>74</v>
+      </c>
+      <c r="M67">
+        <v>3.9642330000000001</v>
+      </c>
+      <c r="N67">
+        <v>99</v>
+      </c>
+      <c r="O67">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="68" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>25</v>
+      </c>
+      <c r="E68">
+        <v>3.6292970000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>26</v>
+      </c>
+      <c r="E69">
+        <v>3.6335190000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>27</v>
+      </c>
+      <c r="E70">
+        <v>3.637324</v>
+      </c>
+    </row>
+    <row r="71" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>28</v>
+      </c>
+      <c r="E71">
+        <v>3.6413039999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>29</v>
+      </c>
+      <c r="E72">
+        <v>3.64567</v>
+      </c>
+    </row>
+    <row r="73" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>30</v>
+      </c>
+      <c r="E73">
+        <v>3.6493099999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>31</v>
+      </c>
+      <c r="E74">
+        <v>3.6531560000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>32</v>
+      </c>
+      <c r="E75">
+        <v>3.6569940000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>33</v>
+      </c>
+      <c r="E76">
+        <v>3.661524</v>
+      </c>
+    </row>
+    <row r="77" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>34</v>
+      </c>
+      <c r="E77">
+        <v>3.6656279999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>35</v>
+      </c>
+      <c r="E78">
+        <v>3.6697329999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>36</v>
+      </c>
+      <c r="E79">
+        <v>3.6741440000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>37</v>
+      </c>
+      <c r="E80">
+        <v>3.6783809999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>38</v>
+      </c>
+      <c r="E81">
+        <v>3.6827390000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>39</v>
+      </c>
+      <c r="E82">
+        <v>3.6873710000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>40</v>
+      </c>
+      <c r="E83">
+        <v>3.6918000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>41</v>
+      </c>
+      <c r="E84">
+        <v>3.6964260000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>42</v>
+      </c>
+      <c r="E85">
+        <v>3.7016909999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>43</v>
+      </c>
+      <c r="E86">
+        <v>3.7068789999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>44</v>
+      </c>
+      <c r="E87">
+        <v>3.7122130000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>45</v>
+      </c>
+      <c r="E88">
+        <v>3.7175470000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>46</v>
+      </c>
+      <c r="E89">
+        <v>3.7231869999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>47</v>
+      </c>
+      <c r="E90">
+        <v>3.729136</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>48</v>
+      </c>
+      <c r="E91">
+        <v>3.735087</v>
+      </c>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>49</v>
+      </c>
+      <c r="E92">
+        <v>3.7408130000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>50</v>
+      </c>
+      <c r="E93">
+        <v>3.7472940000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>51</v>
+      </c>
+      <c r="E94">
+        <v>3.7538320000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>52</v>
+      </c>
+      <c r="E95">
+        <v>3.7604199999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>53</v>
+      </c>
+      <c r="E96">
+        <v>3.7674280000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>54</v>
+      </c>
+      <c r="E97">
+        <v>3.774896</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>55</v>
+      </c>
+      <c r="E98">
+        <v>3.7825730000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>56</v>
+      </c>
+      <c r="E99">
+        <v>3.7906659999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>57</v>
+      </c>
+      <c r="E100">
+        <v>3.7990330000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>58</v>
+      </c>
+      <c r="E101">
+        <v>3.8074910000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>59</v>
+      </c>
+      <c r="E102">
+        <v>3.8157480000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>60</v>
+      </c>
+      <c r="E103">
+        <v>3.8251330000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>61</v>
+      </c>
+      <c r="E104">
+        <v>3.8339430000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>62</v>
+      </c>
+      <c r="E105">
+        <v>3.8435790000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>63</v>
+      </c>
+      <c r="E106">
+        <v>3.8529080000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>64</v>
+      </c>
+      <c r="E107">
+        <v>3.8626680000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>65</v>
+      </c>
+      <c r="E108">
+        <v>3.8725390000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>66</v>
+      </c>
+      <c r="E109">
+        <v>3.8825910000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>67</v>
+      </c>
+      <c r="E110">
+        <v>3.8923559999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>68</v>
+      </c>
+      <c r="E111">
+        <v>3.9026320000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>69</v>
+      </c>
+      <c r="E112">
+        <v>3.9126699999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>70</v>
+      </c>
+      <c r="E113">
+        <v>3.9228160000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>71</v>
+      </c>
+      <c r="E114">
+        <v>3.9329779999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>72</v>
+      </c>
+      <c r="E115">
+        <v>3.9435959999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>73</v>
+      </c>
+      <c r="E116">
+        <v>3.9539240000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>74</v>
+      </c>
+      <c r="E117">
+        <v>3.9642330000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>75</v>
+      </c>
+      <c r="E118">
+        <v>3.9751690000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>76</v>
+      </c>
+      <c r="E119">
+        <v>3.9859170000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>77</v>
+      </c>
+      <c r="E120">
+        <v>3.9967329999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>78</v>
+      </c>
+      <c r="E121">
+        <v>4.0076650000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>79</v>
+      </c>
+      <c r="E122">
+        <v>4.0185440000000003</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>80</v>
+      </c>
+      <c r="E123">
+        <v>4.0295370000000004</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>81</v>
+      </c>
+      <c r="E124">
+        <v>4.041086</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>82</v>
+      </c>
+      <c r="E125">
+        <v>4.0520930000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>83</v>
+      </c>
+      <c r="E126">
+        <v>4.063879</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>84</v>
+      </c>
+      <c r="E127">
+        <v>4.075736</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>85</v>
+      </c>
+      <c r="E128">
+        <v>4.0872869999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>86</v>
+      </c>
+      <c r="E129">
+        <v>4.0992829999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>87</v>
+      </c>
+      <c r="E130">
+        <v>4.1116109999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>88</v>
+      </c>
+      <c r="E131">
+        <v>4.1237729999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>89</v>
+      </c>
+      <c r="E132">
+        <v>4.1360049999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>90</v>
+      </c>
+      <c r="E133">
+        <v>4.1484990000000002</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>91</v>
+      </c>
+      <c r="E134">
+        <v>4.1610300000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>92</v>
+      </c>
+      <c r="E135">
+        <v>4.1737729999999997</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>93</v>
+      </c>
+      <c r="E136">
+        <v>4.1867080000000003</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>94</v>
+      </c>
+      <c r="E137">
+        <v>4.1996310000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>95</v>
+      </c>
+      <c r="E138">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>96</v>
+      </c>
+      <c r="E139">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>97</v>
+      </c>
+      <c r="E140">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>98</v>
+      </c>
+      <c r="E141">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <v>99</v>
+      </c>
+      <c r="E142">
+        <v>4.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>